<commit_message>
Finished the Croston methods
</commit_message>
<xml_diff>
--- a/bip5887_data.xlsx
+++ b/bip5887_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Esteban\TESIS\Tesis\Tesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0359FA64-7127-4D29-9151-302446B08329}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22DC83EB-EFF5-492A-999A-AFD4FF32B213}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{91D287CC-EE7F-49F7-8D19-7A4C550A5EAE}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="5" xr2:uid="{91D287CC-EE7F-49F7-8D19-7A4C550A5EAE}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="0.15" sheetId="3" r:id="rId3"/>
     <sheet name="0.5" sheetId="4" r:id="rId4"/>
     <sheet name="Opt." sheetId="5" r:id="rId5"/>
+    <sheet name="Hoja2" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="67">
   <si>
     <t>X</t>
   </si>
@@ -231,6 +232,15 @@
   <si>
     <t>SBJ (0.15)</t>
   </si>
+  <si>
+    <t>opt</t>
+  </si>
+  <si>
+    <t>Cros.</t>
+  </si>
+  <si>
+    <t>opt.</t>
+  </si>
 </sst>
 </file>
 
@@ -281,7 +291,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -294,6 +304,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -10325,8 +10344,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB63421C-E783-4E38-971A-499FA26892FC}">
   <dimension ref="A1:V43"/>
   <sheetViews>
-    <sheetView topLeftCell="E8" workbookViewId="0">
-      <selection activeCell="Q22" sqref="Q22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="W47" sqref="W47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -14699,7 +14718,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7D29E83-D995-432E-BADE-B18090F1DA3D}">
   <dimension ref="A1:P47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+    <sheetView topLeftCell="A23" workbookViewId="0">
       <selection activeCell="O48" sqref="O48"/>
     </sheetView>
   </sheetViews>
@@ -16172,10 +16191,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3ABCA225-E7BC-489D-B5FC-31296142288C}">
-  <dimension ref="A1:P56"/>
+  <dimension ref="A1:V56"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L33" sqref="L33:P38"/>
+      <selection activeCell="K43" sqref="K43:V44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -17177,7 +17196,7 @@
         <v>-4.9523947169966247</v>
       </c>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>33</v>
       </c>
@@ -17221,7 +17240,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>34</v>
       </c>
@@ -17265,7 +17284,7 @@
         <v>6.0359389999999999E-2</v>
       </c>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>35</v>
       </c>
@@ -17312,7 +17331,7 @@
         <v>0.19759379999999999</v>
       </c>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>36</v>
       </c>
@@ -17359,7 +17378,7 @@
         <v>7.2139457</v>
       </c>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>37</v>
       </c>
@@ -17406,7 +17425,7 @@
         <v>12.4767045</v>
       </c>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:22" x14ac:dyDescent="0.3">
       <c r="C38">
         <v>4.2034789999999997</v>
       </c>
@@ -17439,7 +17458,7 @@
         <v>5.2627588000000003</v>
       </c>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:22" x14ac:dyDescent="0.3">
       <c r="C39">
         <v>4.2034789999999997</v>
       </c>
@@ -17458,7 +17477,7 @@
       <c r="O39" s="6"/>
       <c r="P39" s="6"/>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:22" x14ac:dyDescent="0.3">
       <c r="C40">
         <v>4.2034789999999997</v>
       </c>
@@ -17477,7 +17496,7 @@
       <c r="O40" s="4"/>
       <c r="P40" s="4"/>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:22" x14ac:dyDescent="0.3">
       <c r="C41">
         <v>4.2034789999999997</v>
       </c>
@@ -17496,7 +17515,7 @@
       <c r="O41" s="4"/>
       <c r="P41" s="4"/>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:22" x14ac:dyDescent="0.3">
       <c r="C42">
         <v>4.2034789999999997</v>
       </c>
@@ -17515,42 +17534,88 @@
       <c r="O42" s="4"/>
       <c r="P42" s="4"/>
     </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="L43" s="3"/>
-      <c r="M43" s="4"/>
-      <c r="N43" s="4"/>
-      <c r="O43" s="4"/>
-      <c r="P43" s="4"/>
-    </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="L44" s="3"/>
-      <c r="M44" s="4"/>
-      <c r="N44" s="4"/>
-      <c r="O44" s="4"/>
-      <c r="P44" s="4"/>
-    </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="K43" s="9">
+        <v>0.1</v>
+      </c>
+      <c r="L43" s="9"/>
+      <c r="M43" s="9"/>
+      <c r="N43" s="9">
+        <v>0.15</v>
+      </c>
+      <c r="O43" s="9"/>
+      <c r="P43" s="9"/>
+      <c r="Q43" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="R43" s="9"/>
+      <c r="S43" s="9"/>
+      <c r="T43" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="U43" s="9"/>
+      <c r="V43" s="9"/>
+    </row>
+    <row r="44" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="K44" t="s">
+        <v>65</v>
+      </c>
+      <c r="L44" t="s">
+        <v>40</v>
+      </c>
+      <c r="M44" t="s">
+        <v>41</v>
+      </c>
+      <c r="N44" t="s">
+        <v>65</v>
+      </c>
+      <c r="O44" t="s">
+        <v>40</v>
+      </c>
+      <c r="P44" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q44" t="s">
+        <v>65</v>
+      </c>
+      <c r="R44" t="s">
+        <v>40</v>
+      </c>
+      <c r="S44" t="s">
+        <v>41</v>
+      </c>
+      <c r="T44" t="s">
+        <v>65</v>
+      </c>
+      <c r="U44" t="s">
+        <v>40</v>
+      </c>
+      <c r="V44" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="45" spans="1:22" x14ac:dyDescent="0.3">
       <c r="L45" s="3"/>
       <c r="M45" s="4"/>
       <c r="N45" s="4"/>
       <c r="O45" s="4"/>
       <c r="P45" s="4"/>
     </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:22" x14ac:dyDescent="0.3">
       <c r="L46" s="3"/>
       <c r="M46" s="4"/>
       <c r="N46" s="4"/>
       <c r="O46" s="4"/>
       <c r="P46" s="4"/>
     </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:22" x14ac:dyDescent="0.3">
       <c r="L47" s="3"/>
       <c r="M47" s="4"/>
       <c r="N47" s="4"/>
       <c r="O47" s="4"/>
       <c r="P47" s="4"/>
     </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:22" x14ac:dyDescent="0.3">
       <c r="L48" s="5"/>
       <c r="M48" s="5"/>
       <c r="N48" s="5"/>
@@ -17614,11 +17679,1475 @@
       <c r="P56" s="4"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="6">
+    <mergeCell ref="T43:V43"/>
     <mergeCell ref="L39:P39"/>
     <mergeCell ref="L48:P48"/>
+    <mergeCell ref="K43:M43"/>
+    <mergeCell ref="N43:P43"/>
+    <mergeCell ref="Q43:S43"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB97240C-E9F1-4892-924E-920E90AB7B5F}">
+  <dimension ref="A1:M38"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection sqref="A1:M38"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="7.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="4.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="4.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.21875" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="4.5546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="5.21875" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="4.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B1" s="9">
+        <v>0.1</v>
+      </c>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9">
+        <v>0.15</v>
+      </c>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
+      <c r="K1" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="L1" s="9"/>
+      <c r="M1" s="9"/>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E2" t="s">
+        <v>65</v>
+      </c>
+      <c r="F2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G2" t="s">
+        <v>41</v>
+      </c>
+      <c r="H2" t="s">
+        <v>65</v>
+      </c>
+      <c r="I2" t="s">
+        <v>40</v>
+      </c>
+      <c r="J2" t="s">
+        <v>41</v>
+      </c>
+      <c r="K2" t="s">
+        <v>65</v>
+      </c>
+      <c r="L2" t="s">
+        <v>40</v>
+      </c>
+      <c r="M2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A3" s="7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A4" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A5" s="8">
+        <v>44610</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A6" s="8">
+        <v>44638</v>
+      </c>
+      <c r="B6" s="2">
+        <v>6.5284750000000003</v>
+      </c>
+      <c r="C6" s="2">
+        <v>7.4115060000000001</v>
+      </c>
+      <c r="D6" s="2">
+        <v>7.3884619999999996</v>
+      </c>
+      <c r="E6" s="2">
+        <v>7.9999979999999997</v>
+      </c>
+      <c r="F6" s="2">
+        <v>7.9999950000000002</v>
+      </c>
+      <c r="G6" s="2">
+        <v>7.9999979999999997</v>
+      </c>
+      <c r="H6" s="2">
+        <v>7.9999989999999999</v>
+      </c>
+      <c r="I6" s="2">
+        <v>7.9999979999999997</v>
+      </c>
+      <c r="J6" s="2">
+        <v>7.9999979999999997</v>
+      </c>
+      <c r="K6" s="2">
+        <v>1.000051</v>
+      </c>
+      <c r="L6" s="2">
+        <v>1.0413840000000001</v>
+      </c>
+      <c r="M6" s="2">
+        <v>1.0000020000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A7" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2">
+        <v>6.5284750000000003</v>
+      </c>
+      <c r="C7" s="2">
+        <v>7.4115060000000001</v>
+      </c>
+      <c r="D7" s="2">
+        <v>7.3884619999999996</v>
+      </c>
+      <c r="E7" s="2">
+        <v>7.9999979999999997</v>
+      </c>
+      <c r="F7" s="2">
+        <v>7.9999950000000002</v>
+      </c>
+      <c r="G7" s="2">
+        <v>7.9999979999999997</v>
+      </c>
+      <c r="H7" s="2">
+        <v>7.9999989999999999</v>
+      </c>
+      <c r="I7" s="2">
+        <v>7.9999979999999997</v>
+      </c>
+      <c r="J7" s="2">
+        <v>7.9999979999999997</v>
+      </c>
+      <c r="K7" s="2">
+        <v>1.000051</v>
+      </c>
+      <c r="L7" s="2">
+        <v>1.0413840000000001</v>
+      </c>
+      <c r="M7" s="2">
+        <v>1.0000020000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A8" s="8">
+        <v>44699</v>
+      </c>
+      <c r="B8" s="2">
+        <v>6.075628</v>
+      </c>
+      <c r="C8" s="2">
+        <v>6.870355</v>
+      </c>
+      <c r="D8" s="2">
+        <v>6.8496160000000001</v>
+      </c>
+      <c r="E8" s="2">
+        <v>7.0999990000000004</v>
+      </c>
+      <c r="F8" s="2">
+        <v>7.099996</v>
+      </c>
+      <c r="G8" s="2">
+        <v>7.0999980000000003</v>
+      </c>
+      <c r="H8" s="2">
+        <v>4.9999989999999999</v>
+      </c>
+      <c r="I8" s="2">
+        <v>4.9999989999999999</v>
+      </c>
+      <c r="J8" s="2">
+        <v>4.9999989999999999</v>
+      </c>
+      <c r="K8" s="2">
+        <v>1.0419620000000001</v>
+      </c>
+      <c r="L8" s="2">
+        <v>1.071588</v>
+      </c>
+      <c r="M8" s="2">
+        <v>1.029725</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A9" s="8">
+        <v>44730</v>
+      </c>
+      <c r="B9" s="2">
+        <v>5.5680649999999998</v>
+      </c>
+      <c r="C9" s="2">
+        <v>6.2833199999999998</v>
+      </c>
+      <c r="D9" s="2">
+        <v>6.2646540000000002</v>
+      </c>
+      <c r="E9" s="2">
+        <v>6.1849990000000004</v>
+      </c>
+      <c r="F9" s="2">
+        <v>6.1849970000000001</v>
+      </c>
+      <c r="G9" s="2">
+        <v>6.1849980000000002</v>
+      </c>
+      <c r="H9" s="2">
+        <v>3</v>
+      </c>
+      <c r="I9" s="2">
+        <v>3</v>
+      </c>
+      <c r="J9" s="2">
+        <v>3</v>
+      </c>
+      <c r="K9" s="2">
+        <v>1.040203</v>
+      </c>
+      <c r="L9" s="2">
+        <v>1.0693330000000001</v>
+      </c>
+      <c r="M9" s="2">
+        <v>1.0288409999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A10" s="8">
+        <v>44760</v>
+      </c>
+      <c r="B10" s="2">
+        <v>5.5680649999999998</v>
+      </c>
+      <c r="C10" s="2">
+        <v>6.2833199999999998</v>
+      </c>
+      <c r="D10" s="2">
+        <v>6.2646540000000002</v>
+      </c>
+      <c r="E10" s="2">
+        <v>6.1849990000000004</v>
+      </c>
+      <c r="F10" s="2">
+        <v>6.1849970000000001</v>
+      </c>
+      <c r="G10" s="2">
+        <v>6.1849980000000002</v>
+      </c>
+      <c r="H10" s="2">
+        <v>3</v>
+      </c>
+      <c r="I10" s="2">
+        <v>3</v>
+      </c>
+      <c r="J10" s="2">
+        <v>3</v>
+      </c>
+      <c r="K10" s="2">
+        <v>1.040203</v>
+      </c>
+      <c r="L10" s="2">
+        <v>1.0693330000000001</v>
+      </c>
+      <c r="M10" s="2">
+        <v>1.0288409999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A11" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="2">
+        <v>5.5680649999999998</v>
+      </c>
+      <c r="C11" s="2">
+        <v>6.2833199999999998</v>
+      </c>
+      <c r="D11" s="2">
+        <v>6.2646540000000002</v>
+      </c>
+      <c r="E11" s="2">
+        <v>6.1849990000000004</v>
+      </c>
+      <c r="F11" s="2">
+        <v>6.1849970000000001</v>
+      </c>
+      <c r="G11" s="2">
+        <v>6.1849980000000002</v>
+      </c>
+      <c r="H11" s="2">
+        <v>3</v>
+      </c>
+      <c r="I11" s="2">
+        <v>3</v>
+      </c>
+      <c r="J11" s="2">
+        <v>3</v>
+      </c>
+      <c r="K11" s="2">
+        <v>1.040203</v>
+      </c>
+      <c r="L11" s="2">
+        <v>1.0693330000000001</v>
+      </c>
+      <c r="M11" s="2">
+        <v>1.0288409999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A12" s="8">
+        <v>44822</v>
+      </c>
+      <c r="B12" s="2">
+        <v>5.5680649999999998</v>
+      </c>
+      <c r="C12" s="2">
+        <v>6.2833199999999998</v>
+      </c>
+      <c r="D12" s="2">
+        <v>6.2646540000000002</v>
+      </c>
+      <c r="E12" s="2">
+        <v>6.1849990000000004</v>
+      </c>
+      <c r="F12" s="2">
+        <v>6.1849970000000001</v>
+      </c>
+      <c r="G12" s="2">
+        <v>6.1849980000000002</v>
+      </c>
+      <c r="H12" s="2">
+        <v>3</v>
+      </c>
+      <c r="I12" s="2">
+        <v>3</v>
+      </c>
+      <c r="J12" s="2">
+        <v>3</v>
+      </c>
+      <c r="K12" s="2">
+        <v>1.040203</v>
+      </c>
+      <c r="L12" s="2">
+        <v>1.0693330000000001</v>
+      </c>
+      <c r="M12" s="2">
+        <v>1.0288409999999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A13" s="8">
+        <v>44852</v>
+      </c>
+      <c r="B13" s="2">
+        <v>5.5680649999999998</v>
+      </c>
+      <c r="C13" s="2">
+        <v>6.2833199999999998</v>
+      </c>
+      <c r="D13" s="2">
+        <v>6.2646540000000002</v>
+      </c>
+      <c r="E13" s="2">
+        <v>6.1849990000000004</v>
+      </c>
+      <c r="F13" s="2">
+        <v>6.1849970000000001</v>
+      </c>
+      <c r="G13" s="2">
+        <v>6.1849980000000002</v>
+      </c>
+      <c r="H13" s="2">
+        <v>3</v>
+      </c>
+      <c r="I13" s="2">
+        <v>3</v>
+      </c>
+      <c r="J13" s="2">
+        <v>3</v>
+      </c>
+      <c r="K13" s="2">
+        <v>1.040203</v>
+      </c>
+      <c r="L13" s="2">
+        <v>1.0693330000000001</v>
+      </c>
+      <c r="M13" s="2">
+        <v>1.0288409999999999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A14" s="8">
+        <v>44883</v>
+      </c>
+      <c r="B14" s="2">
+        <v>5.5680649999999998</v>
+      </c>
+      <c r="C14" s="2">
+        <v>6.2833199999999998</v>
+      </c>
+      <c r="D14" s="2">
+        <v>6.2646540000000002</v>
+      </c>
+      <c r="E14" s="2">
+        <v>6.1849990000000004</v>
+      </c>
+      <c r="F14" s="2">
+        <v>6.1849970000000001</v>
+      </c>
+      <c r="G14" s="2">
+        <v>6.1849980000000002</v>
+      </c>
+      <c r="H14" s="2">
+        <v>3</v>
+      </c>
+      <c r="I14" s="2">
+        <v>3</v>
+      </c>
+      <c r="J14" s="2">
+        <v>3</v>
+      </c>
+      <c r="K14" s="2">
+        <v>1.040203</v>
+      </c>
+      <c r="L14" s="2">
+        <v>1.0693330000000001</v>
+      </c>
+      <c r="M14" s="2">
+        <v>1.0288409999999999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A15" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" s="2">
+        <v>5.6112590000000004</v>
+      </c>
+      <c r="C15" s="2">
+        <v>6.254988</v>
+      </c>
+      <c r="D15" s="2">
+        <v>6.2381890000000002</v>
+      </c>
+      <c r="E15" s="2">
+        <v>6.1572490000000002</v>
+      </c>
+      <c r="F15" s="2">
+        <v>6.1572469999999999</v>
+      </c>
+      <c r="G15" s="2">
+        <v>6.1572480000000001</v>
+      </c>
+      <c r="H15" s="2">
+        <v>4.5</v>
+      </c>
+      <c r="I15" s="2">
+        <v>4.5</v>
+      </c>
+      <c r="J15" s="2">
+        <v>4.5</v>
+      </c>
+      <c r="K15" s="2">
+        <v>1.248081</v>
+      </c>
+      <c r="L15" s="2">
+        <v>1.2246889999999999</v>
+      </c>
+      <c r="M15" s="2">
+        <v>1.176601</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A16" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" s="2">
+        <v>5.6112590000000004</v>
+      </c>
+      <c r="C16" s="2">
+        <v>6.254988</v>
+      </c>
+      <c r="D16" s="2">
+        <v>6.2381890000000002</v>
+      </c>
+      <c r="E16" s="2">
+        <v>6.1572490000000002</v>
+      </c>
+      <c r="F16" s="2">
+        <v>6.1572469999999999</v>
+      </c>
+      <c r="G16" s="2">
+        <v>6.1572480000000001</v>
+      </c>
+      <c r="H16" s="2">
+        <v>4.5</v>
+      </c>
+      <c r="I16" s="2">
+        <v>4.5</v>
+      </c>
+      <c r="J16" s="2">
+        <v>4.5</v>
+      </c>
+      <c r="K16" s="2">
+        <v>1.248081</v>
+      </c>
+      <c r="L16" s="2">
+        <v>1.2246889999999999</v>
+      </c>
+      <c r="M16" s="2">
+        <v>1.176601</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A17" s="8">
+        <v>44611</v>
+      </c>
+      <c r="B17" s="2">
+        <v>5.6112590000000004</v>
+      </c>
+      <c r="C17" s="2">
+        <v>6.254988</v>
+      </c>
+      <c r="D17" s="2">
+        <v>6.2381890000000002</v>
+      </c>
+      <c r="E17" s="2">
+        <v>6.1572490000000002</v>
+      </c>
+      <c r="F17" s="2">
+        <v>6.1572469999999999</v>
+      </c>
+      <c r="G17" s="2">
+        <v>6.1572480000000001</v>
+      </c>
+      <c r="H17" s="2">
+        <v>4.5</v>
+      </c>
+      <c r="I17" s="2">
+        <v>4.5</v>
+      </c>
+      <c r="J17" s="2">
+        <v>4.5</v>
+      </c>
+      <c r="K17" s="2">
+        <v>1.248081</v>
+      </c>
+      <c r="L17" s="2">
+        <v>1.2246889999999999</v>
+      </c>
+      <c r="M17" s="2">
+        <v>1.176601</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A18" s="8">
+        <v>44639</v>
+      </c>
+      <c r="B18" s="2">
+        <v>5.6112590000000004</v>
+      </c>
+      <c r="C18" s="2">
+        <v>6.254988</v>
+      </c>
+      <c r="D18" s="2">
+        <v>6.2381890000000002</v>
+      </c>
+      <c r="E18" s="2">
+        <v>6.1572490000000002</v>
+      </c>
+      <c r="F18" s="2">
+        <v>6.1572469999999999</v>
+      </c>
+      <c r="G18" s="2">
+        <v>6.1572480000000001</v>
+      </c>
+      <c r="H18" s="2">
+        <v>4.5</v>
+      </c>
+      <c r="I18" s="2">
+        <v>4.5</v>
+      </c>
+      <c r="J18" s="2">
+        <v>4.5</v>
+      </c>
+      <c r="K18" s="2">
+        <v>1.248081</v>
+      </c>
+      <c r="L18" s="2">
+        <v>1.2246889999999999</v>
+      </c>
+      <c r="M18" s="2">
+        <v>1.176601</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A19" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B19" s="2">
+        <v>5.4501330000000001</v>
+      </c>
+      <c r="C19" s="2">
+        <v>6.0294889999999999</v>
+      </c>
+      <c r="D19" s="2">
+        <v>6.0143700000000004</v>
+      </c>
+      <c r="E19" s="2">
+        <v>5.8336620000000003</v>
+      </c>
+      <c r="F19" s="2">
+        <v>5.8336600000000001</v>
+      </c>
+      <c r="G19" s="2">
+        <v>5.8336610000000002</v>
+      </c>
+      <c r="H19" s="2">
+        <v>4.25</v>
+      </c>
+      <c r="I19" s="2">
+        <v>4.25</v>
+      </c>
+      <c r="J19" s="2">
+        <v>4.25</v>
+      </c>
+      <c r="K19" s="2">
+        <v>1.363421</v>
+      </c>
+      <c r="L19" s="2">
+        <v>1.3121339999999999</v>
+      </c>
+      <c r="M19" s="2">
+        <v>1.260521</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A20" s="8">
+        <v>44700</v>
+      </c>
+      <c r="B20" s="2">
+        <v>5.0051189999999997</v>
+      </c>
+      <c r="C20" s="2">
+        <v>5.5265399999999998</v>
+      </c>
+      <c r="D20" s="2">
+        <v>5.5129330000000003</v>
+      </c>
+      <c r="E20" s="2">
+        <v>5.1086119999999999</v>
+      </c>
+      <c r="F20" s="2">
+        <v>5.1086109999999998</v>
+      </c>
+      <c r="G20" s="2">
+        <v>5.1086119999999999</v>
+      </c>
+      <c r="H20" s="2">
+        <v>2.625</v>
+      </c>
+      <c r="I20" s="2">
+        <v>2.625</v>
+      </c>
+      <c r="J20" s="2">
+        <v>2.625</v>
+      </c>
+      <c r="K20" s="2">
+        <v>1.3481890000000001</v>
+      </c>
+      <c r="L20" s="2">
+        <v>1.3022990000000001</v>
+      </c>
+      <c r="M20" s="2">
+        <v>1.2527779999999999</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A21" s="8">
+        <v>44731</v>
+      </c>
+      <c r="B21" s="2">
+        <v>5.0051189999999997</v>
+      </c>
+      <c r="C21" s="2">
+        <v>5.5265399999999998</v>
+      </c>
+      <c r="D21" s="2">
+        <v>5.5129330000000003</v>
+      </c>
+      <c r="E21" s="2">
+        <v>5.1086119999999999</v>
+      </c>
+      <c r="F21" s="2">
+        <v>5.1086109999999998</v>
+      </c>
+      <c r="G21" s="2">
+        <v>5.1086119999999999</v>
+      </c>
+      <c r="H21" s="2">
+        <v>2.625</v>
+      </c>
+      <c r="I21" s="2">
+        <v>2.625</v>
+      </c>
+      <c r="J21" s="2">
+        <v>2.625</v>
+      </c>
+      <c r="K21" s="2">
+        <v>1.3481890000000001</v>
+      </c>
+      <c r="L21" s="2">
+        <v>1.3022990000000001</v>
+      </c>
+      <c r="M21" s="2">
+        <v>1.2527779999999999</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A22" s="8">
+        <v>44761</v>
+      </c>
+      <c r="B22" s="2">
+        <v>4.7046080000000003</v>
+      </c>
+      <c r="C22" s="2">
+        <v>5.1738860000000004</v>
+      </c>
+      <c r="D22" s="2">
+        <v>5.1616400000000002</v>
+      </c>
+      <c r="E22" s="2">
+        <v>4.6423199999999998</v>
+      </c>
+      <c r="F22" s="2">
+        <v>4.6423189999999996</v>
+      </c>
+      <c r="G22" s="2">
+        <v>4.6423199999999998</v>
+      </c>
+      <c r="H22" s="2">
+        <v>2.3125</v>
+      </c>
+      <c r="I22" s="2">
+        <v>2.3125</v>
+      </c>
+      <c r="J22" s="2">
+        <v>2.3125</v>
+      </c>
+      <c r="K22" s="2">
+        <v>1.375508</v>
+      </c>
+      <c r="L22" s="2">
+        <v>1.324282</v>
+      </c>
+      <c r="M22" s="2">
+        <v>1.274988</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A23" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B23" s="2">
+        <v>4.3341469999999997</v>
+      </c>
+      <c r="C23" s="2">
+        <v>4.7564970000000004</v>
+      </c>
+      <c r="D23" s="2">
+        <v>4.745476</v>
+      </c>
+      <c r="E23" s="2">
+        <v>4.0959719999999997</v>
+      </c>
+      <c r="F23" s="2">
+        <v>4.0959719999999997</v>
+      </c>
+      <c r="G23" s="2">
+        <v>4.0959719999999997</v>
+      </c>
+      <c r="H23" s="2">
+        <v>1.65625</v>
+      </c>
+      <c r="I23" s="2">
+        <v>1.65625</v>
+      </c>
+      <c r="J23" s="2">
+        <v>1.65625</v>
+      </c>
+      <c r="K23" s="2">
+        <v>1.3597699999999999</v>
+      </c>
+      <c r="L23" s="2">
+        <v>1.314065</v>
+      </c>
+      <c r="M23" s="2">
+        <v>1.2668140000000001</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A24" s="8">
+        <v>44823</v>
+      </c>
+      <c r="B24" s="2">
+        <v>4.0007320000000002</v>
+      </c>
+      <c r="C24" s="2">
+        <v>4.3808480000000003</v>
+      </c>
+      <c r="D24" s="2">
+        <v>4.3709280000000001</v>
+      </c>
+      <c r="E24" s="2">
+        <v>3.6315770000000001</v>
+      </c>
+      <c r="F24" s="2">
+        <v>3.6315759999999999</v>
+      </c>
+      <c r="G24" s="2">
+        <v>3.6315759999999999</v>
+      </c>
+      <c r="H24" s="2">
+        <v>1.328125</v>
+      </c>
+      <c r="I24" s="2">
+        <v>1.328125</v>
+      </c>
+      <c r="J24" s="2">
+        <v>1.328125</v>
+      </c>
+      <c r="K24" s="2">
+        <v>1.3446910000000001</v>
+      </c>
+      <c r="L24" s="2">
+        <v>1.3041689999999999</v>
+      </c>
+      <c r="M24" s="2">
+        <v>1.2588839999999999</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A25" s="8">
+        <v>44853</v>
+      </c>
+      <c r="B25" s="2">
+        <v>3.7006589999999999</v>
+      </c>
+      <c r="C25" s="2">
+        <v>4.0427629999999999</v>
+      </c>
+      <c r="D25" s="2">
+        <v>4.0338349999999998</v>
+      </c>
+      <c r="E25" s="2">
+        <v>3.2368399999999999</v>
+      </c>
+      <c r="F25" s="2">
+        <v>3.2368389999999998</v>
+      </c>
+      <c r="G25" s="2">
+        <v>3.2368399999999999</v>
+      </c>
+      <c r="H25" s="2">
+        <v>1.1640619999999999</v>
+      </c>
+      <c r="I25" s="2">
+        <v>1.1640619999999999</v>
+      </c>
+      <c r="J25" s="2">
+        <v>1.1640619999999999</v>
+      </c>
+      <c r="K25" s="2">
+        <v>1.330244</v>
+      </c>
+      <c r="L25" s="2">
+        <v>1.2945850000000001</v>
+      </c>
+      <c r="M25" s="2">
+        <v>1.2511890000000001</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A26" s="8">
+        <v>44884</v>
+      </c>
+      <c r="B26" s="2">
+        <v>3.430593</v>
+      </c>
+      <c r="C26" s="2">
+        <v>3.7384870000000001</v>
+      </c>
+      <c r="D26" s="2">
+        <v>3.7304520000000001</v>
+      </c>
+      <c r="E26" s="2">
+        <v>2.9013140000000002</v>
+      </c>
+      <c r="F26" s="2">
+        <v>2.9013140000000002</v>
+      </c>
+      <c r="G26" s="2">
+        <v>2.9013140000000002</v>
+      </c>
+      <c r="H26" s="2">
+        <v>1.082031</v>
+      </c>
+      <c r="I26" s="2">
+        <v>1.082031</v>
+      </c>
+      <c r="J26" s="2">
+        <v>1.082031</v>
+      </c>
+      <c r="K26" s="2">
+        <v>1.3164020000000001</v>
+      </c>
+      <c r="L26" s="2">
+        <v>1.285304</v>
+      </c>
+      <c r="M26" s="2">
+        <v>1.2437229999999999</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A27" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B27" s="2">
+        <v>3.1875339999999999</v>
+      </c>
+      <c r="C27" s="2">
+        <v>3.4646379999999999</v>
+      </c>
+      <c r="D27" s="2">
+        <v>3.4574069999999999</v>
+      </c>
+      <c r="E27" s="2">
+        <v>2.616117</v>
+      </c>
+      <c r="F27" s="2">
+        <v>2.6161159999999999</v>
+      </c>
+      <c r="G27" s="2">
+        <v>2.616117</v>
+      </c>
+      <c r="H27" s="2">
+        <v>1.0410159999999999</v>
+      </c>
+      <c r="I27" s="2">
+        <v>1.0410159999999999</v>
+      </c>
+      <c r="J27" s="2">
+        <v>1.0410159999999999</v>
+      </c>
+      <c r="K27" s="2">
+        <v>1.3031410000000001</v>
+      </c>
+      <c r="L27" s="2">
+        <v>1.2763139999999999</v>
+      </c>
+      <c r="M27" s="2">
+        <v>1.236478</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A28" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B28" s="2">
+        <v>3.1875339999999999</v>
+      </c>
+      <c r="C28" s="2">
+        <v>3.4646379999999999</v>
+      </c>
+      <c r="D28" s="2">
+        <v>3.4574069999999999</v>
+      </c>
+      <c r="E28" s="2">
+        <v>2.616117</v>
+      </c>
+      <c r="F28" s="2">
+        <v>2.6161159999999999</v>
+      </c>
+      <c r="G28" s="2">
+        <v>2.616117</v>
+      </c>
+      <c r="H28" s="2">
+        <v>1.0410159999999999</v>
+      </c>
+      <c r="I28" s="2">
+        <v>1.0410159999999999</v>
+      </c>
+      <c r="J28" s="2">
+        <v>1.0410159999999999</v>
+      </c>
+      <c r="K28" s="2">
+        <v>1.3031410000000001</v>
+      </c>
+      <c r="L28" s="2">
+        <v>1.2763139999999999</v>
+      </c>
+      <c r="M28" s="2">
+        <v>1.236478</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A29" s="8">
+        <v>44612</v>
+      </c>
+      <c r="B29" s="2">
+        <v>3.0687799999999998</v>
+      </c>
+      <c r="C29" s="2">
+        <v>3.318174</v>
+      </c>
+      <c r="D29" s="2">
+        <v>3.3116660000000002</v>
+      </c>
+      <c r="E29" s="2">
+        <v>2.5236990000000001</v>
+      </c>
+      <c r="F29" s="2">
+        <v>2.5236990000000001</v>
+      </c>
+      <c r="G29" s="2">
+        <v>2.5236990000000001</v>
+      </c>
+      <c r="H29" s="2">
+        <v>1.520508</v>
+      </c>
+      <c r="I29" s="2">
+        <v>1.520508</v>
+      </c>
+      <c r="J29" s="2">
+        <v>1.520508</v>
+      </c>
+      <c r="K29" s="2">
+        <v>1.3323480000000001</v>
+      </c>
+      <c r="L29" s="2">
+        <v>1.2991159999999999</v>
+      </c>
+      <c r="M29" s="2">
+        <v>1.2591730000000001</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A30" s="8">
+        <v>44640</v>
+      </c>
+      <c r="B30" s="2">
+        <v>2.8619020000000002</v>
+      </c>
+      <c r="C30" s="2">
+        <v>3.086357</v>
+      </c>
+      <c r="D30" s="2">
+        <v>3.0804990000000001</v>
+      </c>
+      <c r="E30" s="2">
+        <v>2.2951440000000001</v>
+      </c>
+      <c r="F30" s="2">
+        <v>2.2951440000000001</v>
+      </c>
+      <c r="G30" s="2">
+        <v>2.2951440000000001</v>
+      </c>
+      <c r="H30" s="2">
+        <v>1.260254</v>
+      </c>
+      <c r="I30" s="2">
+        <v>1.260254</v>
+      </c>
+      <c r="J30" s="2">
+        <v>1.260254</v>
+      </c>
+      <c r="K30" s="2">
+        <v>1.318419</v>
+      </c>
+      <c r="L30" s="2">
+        <v>1.2896920000000001</v>
+      </c>
+      <c r="M30" s="2">
+        <v>1.2514689999999999</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A31" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B31" s="2">
+        <v>2.8619020000000002</v>
+      </c>
+      <c r="C31" s="2">
+        <v>3.086357</v>
+      </c>
+      <c r="D31" s="2">
+        <v>3.0804990000000001</v>
+      </c>
+      <c r="E31" s="2">
+        <v>2.2951440000000001</v>
+      </c>
+      <c r="F31" s="2">
+        <v>2.2951440000000001</v>
+      </c>
+      <c r="G31" s="2">
+        <v>2.2951440000000001</v>
+      </c>
+      <c r="H31" s="2">
+        <v>1.260254</v>
+      </c>
+      <c r="I31" s="2">
+        <v>1.260254</v>
+      </c>
+      <c r="J31" s="2">
+        <v>1.260254</v>
+      </c>
+      <c r="K31" s="2">
+        <v>1.318419</v>
+      </c>
+      <c r="L31" s="2">
+        <v>1.2896920000000001</v>
+      </c>
+      <c r="M31" s="2">
+        <v>1.2514689999999999</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A32" s="8">
+        <v>44701</v>
+      </c>
+      <c r="B32" s="2">
+        <v>2.8619020000000002</v>
+      </c>
+      <c r="C32" s="2">
+        <v>3.086357</v>
+      </c>
+      <c r="D32" s="2">
+        <v>3.0804990000000001</v>
+      </c>
+      <c r="E32" s="2">
+        <v>2.2951440000000001</v>
+      </c>
+      <c r="F32" s="2">
+        <v>2.2951440000000001</v>
+      </c>
+      <c r="G32" s="2">
+        <v>2.2951440000000001</v>
+      </c>
+      <c r="H32" s="2">
+        <v>1.260254</v>
+      </c>
+      <c r="I32" s="2">
+        <v>1.260254</v>
+      </c>
+      <c r="J32" s="2">
+        <v>1.260254</v>
+      </c>
+      <c r="K32" s="2">
+        <v>1.318419</v>
+      </c>
+      <c r="L32" s="2">
+        <v>1.2896920000000001</v>
+      </c>
+      <c r="M32" s="2">
+        <v>1.2514689999999999</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A33" s="8">
+        <v>44732</v>
+      </c>
+      <c r="B33" s="2">
+        <v>2.8619020000000002</v>
+      </c>
+      <c r="C33" s="2">
+        <v>3.086357</v>
+      </c>
+      <c r="D33" s="2">
+        <v>3.0804990000000001</v>
+      </c>
+      <c r="E33" s="2">
+        <v>2.2951440000000001</v>
+      </c>
+      <c r="F33" s="2">
+        <v>2.2951440000000001</v>
+      </c>
+      <c r="G33" s="2">
+        <v>2.2951440000000001</v>
+      </c>
+      <c r="H33" s="2">
+        <v>1.260254</v>
+      </c>
+      <c r="I33" s="2">
+        <v>1.260254</v>
+      </c>
+      <c r="J33" s="2">
+        <v>1.260254</v>
+      </c>
+      <c r="K33" s="2">
+        <v>1.318419</v>
+      </c>
+      <c r="L33" s="2">
+        <v>1.2896920000000001</v>
+      </c>
+      <c r="M33" s="2">
+        <v>1.2514689999999999</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A34" s="8">
+        <v>44762</v>
+      </c>
+      <c r="B34" s="2">
+        <v>2.8619020000000002</v>
+      </c>
+      <c r="C34" s="2">
+        <v>3.086357</v>
+      </c>
+      <c r="D34" s="2">
+        <v>3.0804990000000001</v>
+      </c>
+      <c r="E34" s="2">
+        <v>2.2951440000000001</v>
+      </c>
+      <c r="F34" s="2">
+        <v>2.2951440000000001</v>
+      </c>
+      <c r="G34" s="2">
+        <v>2.2951440000000001</v>
+      </c>
+      <c r="H34" s="2">
+        <v>1.260254</v>
+      </c>
+      <c r="I34" s="2">
+        <v>1.260254</v>
+      </c>
+      <c r="J34" s="2">
+        <v>1.260254</v>
+      </c>
+      <c r="K34" s="2">
+        <v>1.318419</v>
+      </c>
+      <c r="L34" s="2">
+        <v>1.2896920000000001</v>
+      </c>
+      <c r="M34" s="2">
+        <v>1.2514689999999999</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A35" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B35" s="2">
+        <v>2.8619020000000002</v>
+      </c>
+      <c r="C35" s="2">
+        <v>3.086357</v>
+      </c>
+      <c r="D35" s="2">
+        <v>3.0804990000000001</v>
+      </c>
+      <c r="E35" s="2">
+        <v>2.2951440000000001</v>
+      </c>
+      <c r="F35" s="2">
+        <v>2.2951440000000001</v>
+      </c>
+      <c r="G35" s="2">
+        <v>2.2951440000000001</v>
+      </c>
+      <c r="H35" s="2">
+        <v>1.260254</v>
+      </c>
+      <c r="I35" s="2">
+        <v>1.260254</v>
+      </c>
+      <c r="J35" s="2">
+        <v>1.260254</v>
+      </c>
+      <c r="K35" s="2">
+        <v>1.318419</v>
+      </c>
+      <c r="L35" s="2">
+        <v>1.2896920000000001</v>
+      </c>
+      <c r="M35" s="2">
+        <v>1.2514689999999999</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A36" s="8">
+        <v>44824</v>
+      </c>
+      <c r="B36" s="2">
+        <v>2.8619020000000002</v>
+      </c>
+      <c r="C36" s="2">
+        <v>3.086357</v>
+      </c>
+      <c r="D36" s="2">
+        <v>3.0804990000000001</v>
+      </c>
+      <c r="E36" s="2">
+        <v>2.2951440000000001</v>
+      </c>
+      <c r="F36" s="2">
+        <v>2.2951440000000001</v>
+      </c>
+      <c r="G36" s="2">
+        <v>2.2951440000000001</v>
+      </c>
+      <c r="H36" s="2">
+        <v>1.260254</v>
+      </c>
+      <c r="I36" s="2">
+        <v>1.260254</v>
+      </c>
+      <c r="J36" s="2">
+        <v>1.260254</v>
+      </c>
+      <c r="K36" s="2">
+        <v>1.318419</v>
+      </c>
+      <c r="L36" s="2">
+        <v>1.2896920000000001</v>
+      </c>
+      <c r="M36" s="2">
+        <v>1.2514689999999999</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A37" s="8">
+        <v>44854</v>
+      </c>
+      <c r="B37" s="2">
+        <v>2.8619020000000002</v>
+      </c>
+      <c r="C37" s="2">
+        <v>3.086357</v>
+      </c>
+      <c r="D37" s="2">
+        <v>3.0804990000000001</v>
+      </c>
+      <c r="E37" s="2">
+        <v>2.2951440000000001</v>
+      </c>
+      <c r="F37" s="2">
+        <v>2.2951440000000001</v>
+      </c>
+      <c r="G37" s="2">
+        <v>2.2951440000000001</v>
+      </c>
+      <c r="H37" s="2">
+        <v>1.260254</v>
+      </c>
+      <c r="I37" s="2">
+        <v>1.260254</v>
+      </c>
+      <c r="J37" s="2">
+        <v>1.260254</v>
+      </c>
+      <c r="K37" s="2">
+        <v>1.318419</v>
+      </c>
+      <c r="L37" s="2">
+        <v>1.2896920000000001</v>
+      </c>
+      <c r="M37" s="2">
+        <v>1.2514689999999999</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A38" s="8">
+        <v>44885</v>
+      </c>
+      <c r="B38" s="2">
+        <v>3.375712</v>
+      </c>
+      <c r="C38" s="2">
+        <v>3.5777209999999999</v>
+      </c>
+      <c r="D38" s="2">
+        <v>3.5724490000000002</v>
+      </c>
+      <c r="E38" s="2">
+        <v>3.1508729999999998</v>
+      </c>
+      <c r="F38" s="2">
+        <v>3.1508729999999998</v>
+      </c>
+      <c r="G38" s="2">
+        <v>3.1508729999999998</v>
+      </c>
+      <c r="H38" s="2">
+        <v>4.6301269999999999</v>
+      </c>
+      <c r="I38" s="2">
+        <v>4.6301269999999999</v>
+      </c>
+      <c r="J38" s="2">
+        <v>4.6301269999999999</v>
+      </c>
+      <c r="K38" s="2">
+        <v>1.5984609999999999</v>
+      </c>
+      <c r="L38" s="2">
+        <v>1.5011209999999999</v>
+      </c>
+      <c r="M38" s="2">
+        <v>1.4520580000000001</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="H1:J1"/>
+    <mergeCell ref="K1:M1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Finished chapter 5 and Annexes
</commit_message>
<xml_diff>
--- a/bip5887_data.xlsx
+++ b/bip5887_data.xlsx
@@ -506,7 +506,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5162,7 +5161,7 @@
             <c:numRef>
               <c:f>'0.1'!$C$2:$C$42</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="41"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
@@ -5455,7 +5454,7 @@
             <c:numRef>
               <c:f>'0.1'!$D$2:$D$42</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="41"/>
                 <c:pt idx="3">
                   <c:v>5.3073741064902578</c:v>
@@ -5739,7 +5738,7 @@
             <c:numRef>
               <c:f>'0.1'!$E$2:$E$42</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="41"/>
                 <c:pt idx="3">
                   <c:v>5.3790333434146422</c:v>
@@ -6023,7 +6022,7 @@
             <c:numRef>
               <c:f>'0.1'!$F$2:$F$42</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="41"/>
                 <c:pt idx="3">
                   <c:v>5.3826309192012474</c:v>
@@ -7148,7 +7147,7 @@
             <c:numRef>
               <c:f>'0.15'!$C$2:$C$42</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="41"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
@@ -7441,7 +7440,7 @@
             <c:numRef>
               <c:f>'0.15'!$D$2:$D$42</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="41"/>
                 <c:pt idx="3">
                   <c:v>4.8942440594470114</c:v>
@@ -7725,7 +7724,7 @@
             <c:numRef>
               <c:f>'0.15'!$E$2:$E$42</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="41"/>
                 <c:pt idx="3">
                   <c:v>5.1464625281898337</c:v>
@@ -8009,7 +8008,7 @@
             <c:numRef>
               <c:f>'0.15'!$F$2:$F$42</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="41"/>
                 <c:pt idx="3">
                   <c:v>5.1559946109209687</c:v>
@@ -8856,9 +8855,9 @@
             <c:numRef>
               <c:f>'0.5'!$C$2:$C$42</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="41"/>
-                <c:pt idx="0">
+                <c:pt idx="0" formatCode="General">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
@@ -9149,7 +9148,7 @@
             <c:numRef>
               <c:f>'0.5'!$D$2:$D$42</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="41"/>
                 <c:pt idx="3">
                   <c:v>3.4673832482421782E-5</c:v>
@@ -9433,7 +9432,7 @@
             <c:numRef>
               <c:f>'0.5'!$E$2:$E$42</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="41"/>
                 <c:pt idx="3">
                   <c:v>1.5681488620568459E-4</c:v>
@@ -9717,7 +9716,7 @@
             <c:numRef>
               <c:f>'0.5'!$F$2:$F$42</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="41"/>
                 <c:pt idx="3">
                   <c:v>1.3939100996060861E-4</c:v>
@@ -10286,7 +10285,7 @@
             <c:numRef>
               <c:f>Opt.!$B$2:$B$42</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="41"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
@@ -10564,7 +10563,7 @@
             <c:numRef>
               <c:f>Opt.!$C$2:$C$42</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="41"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
@@ -10857,7 +10856,7 @@
             <c:numRef>
               <c:f>Opt.!$D$2:$D$42</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="41"/>
                 <c:pt idx="3">
                   <c:v>1.7486934390646469</c:v>
@@ -11141,7 +11140,7 @@
             <c:numRef>
               <c:f>Opt.!$E$2:$E$42</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="41"/>
                 <c:pt idx="3">
                   <c:v>2.4117076579132268</c:v>
@@ -11425,7 +11424,7 @@
             <c:numRef>
               <c:f>Opt.!$F$2:$F$42</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="41"/>
                 <c:pt idx="3">
                   <c:v>2.6457967397043669</c:v>
@@ -11636,7 +11635,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -12256,115 +12255,115 @@
                 <c:pt idx="3">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="4" formatCode="0.00">
                   <c:v>1.0783389999999999</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="5" formatCode="0.00">
                   <c:v>1.0783389999999999</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="6" formatCode="0.00">
                   <c:v>6.1666910000000001</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="7" formatCode="0.00">
                   <c:v>6.1666910000000001</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="8" formatCode="0.00">
                   <c:v>6.1666910000000001</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="9" formatCode="0.00">
                   <c:v>6.1666910000000001</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="10" formatCode="0.00">
                   <c:v>6.1666910000000001</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="11" formatCode="0.00">
                   <c:v>6.1666910000000001</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="12" formatCode="0.00">
                   <c:v>5.1895519999999999</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="13" formatCode="0.00">
                   <c:v>5.1895519999999999</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="14" formatCode="0.00">
                   <c:v>5.1895519999999999</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="15" formatCode="0.00">
                   <c:v>5.1895519999999999</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="16" formatCode="0.00">
                   <c:v>4.4738360000000004</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="17" formatCode="0.00">
                   <c:v>4.4738360000000004</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="18" formatCode="0.00">
                   <c:v>4.5093719999999999</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="19" formatCode="0.00">
                   <c:v>4.5093719999999999</c:v>
                 </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="20" formatCode="0.00">
                   <c:v>7.6817570000000002</c:v>
                 </c:pt>
-                <c:pt idx="21">
+                <c:pt idx="21" formatCode="0.00">
                   <c:v>7.6817570000000002</c:v>
                 </c:pt>
-                <c:pt idx="22">
+                <c:pt idx="22" formatCode="0.00">
                   <c:v>8.1427560000000003</c:v>
                 </c:pt>
-                <c:pt idx="23">
+                <c:pt idx="23" formatCode="0.00">
                   <c:v>8.1427560000000003</c:v>
                 </c:pt>
-                <c:pt idx="24">
+                <c:pt idx="24" formatCode="0.00">
                   <c:v>7.0483010000000004</c:v>
                 </c:pt>
-                <c:pt idx="25">
+                <c:pt idx="25" formatCode="0.00">
                   <c:v>7.0483010000000004</c:v>
                 </c:pt>
-                <c:pt idx="26">
+                <c:pt idx="26" formatCode="0.00">
                   <c:v>6.1401979999999998</c:v>
                 </c:pt>
-                <c:pt idx="27">
+                <c:pt idx="27" formatCode="0.00">
                   <c:v>6.1401979999999998</c:v>
                 </c:pt>
-                <c:pt idx="28">
+                <c:pt idx="28" formatCode="0.00">
                   <c:v>5.84375</c:v>
                 </c:pt>
-                <c:pt idx="29">
+                <c:pt idx="29" formatCode="0.00">
                   <c:v>5.84375</c:v>
                 </c:pt>
-                <c:pt idx="30">
+                <c:pt idx="30" formatCode="0.00">
                   <c:v>5.84375</c:v>
                 </c:pt>
-                <c:pt idx="31">
+                <c:pt idx="31" formatCode="0.00">
                   <c:v>5.84375</c:v>
                 </c:pt>
-                <c:pt idx="32">
+                <c:pt idx="32" formatCode="0.00">
                   <c:v>5.84375</c:v>
                 </c:pt>
-                <c:pt idx="33">
+                <c:pt idx="33" formatCode="0.00">
                   <c:v>5.84375</c:v>
                 </c:pt>
-                <c:pt idx="34">
+                <c:pt idx="34" formatCode="0.00">
                   <c:v>5.84375</c:v>
                 </c:pt>
-                <c:pt idx="35">
+                <c:pt idx="35" formatCode="0.00">
                   <c:v>5.84375</c:v>
                 </c:pt>
-                <c:pt idx="36">
+                <c:pt idx="36" formatCode="0.00">
                   <c:v>4.9694890000000003</c:v>
                 </c:pt>
-                <c:pt idx="37">
+                <c:pt idx="37" formatCode="0.00">
                   <c:v>4.9694890000000003</c:v>
                 </c:pt>
-                <c:pt idx="38">
+                <c:pt idx="38" formatCode="0.00">
                   <c:v>4.9694890000000003</c:v>
                 </c:pt>
-                <c:pt idx="39">
+                <c:pt idx="39" formatCode="0.00">
                   <c:v>4.9694890000000003</c:v>
                 </c:pt>
-                <c:pt idx="40">
+                <c:pt idx="40" formatCode="0.00">
                   <c:v>4.9694890000000003</c:v>
                 </c:pt>
               </c:numCache>
@@ -12433,115 +12432,115 @@
                 <c:pt idx="3">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="4">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="4" formatCode="0.00">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="0.00">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6" formatCode="0.00">
                   <c:v>5.852176</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="7" formatCode="0.00">
                   <c:v>5.852176</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="8" formatCode="0.00">
                   <c:v>6.147691</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="9" formatCode="0.00">
                   <c:v>6.1698870000000001</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="10" formatCode="0.00">
                   <c:v>6.1698870000000001</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="11" formatCode="0.00">
                   <c:v>6.1698870000000001</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="12" formatCode="0.00">
                   <c:v>5.6762990000000002</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="13" formatCode="0.00">
                   <c:v>5.6762990000000002</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="14" formatCode="0.00">
                   <c:v>5.6762990000000002</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="15" formatCode="0.00">
                   <c:v>5.6269609999999997</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="16" formatCode="0.00">
                   <c:v>5.2961749999999999</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="17" formatCode="0.00">
                   <c:v>5.3348389999999997</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="18" formatCode="0.00">
                   <c:v>5.2795180000000004</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="19" formatCode="0.00">
                   <c:v>5.2196829999999999</c:v>
                 </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="20" formatCode="0.00">
                   <c:v>6.2039920000000004</c:v>
                 </c:pt>
-                <c:pt idx="21">
+                <c:pt idx="21" formatCode="0.00">
                   <c:v>6.997306</c:v>
                 </c:pt>
-                <c:pt idx="22">
+                <c:pt idx="22" formatCode="0.00">
                   <c:v>7.0972309999999998</c:v>
                 </c:pt>
-                <c:pt idx="23">
+                <c:pt idx="23" formatCode="0.00">
                   <c:v>7.0252790000000003</c:v>
                 </c:pt>
-                <c:pt idx="24">
+                <c:pt idx="24" formatCode="0.00">
                   <c:v>6.5723950000000002</c:v>
                 </c:pt>
-                <c:pt idx="25">
+                <c:pt idx="25" formatCode="0.00">
                   <c:v>6.5723950000000002</c:v>
                 </c:pt>
-                <c:pt idx="26">
+                <c:pt idx="26" formatCode="0.00">
                   <c:v>6.3916950000000003</c:v>
                 </c:pt>
-                <c:pt idx="27">
+                <c:pt idx="27" formatCode="0.00">
                   <c:v>6.3611769999999996</c:v>
                 </c:pt>
-                <c:pt idx="28">
+                <c:pt idx="28" formatCode="0.00">
                   <c:v>5.9639629999999997</c:v>
                 </c:pt>
-                <c:pt idx="29">
+                <c:pt idx="29" formatCode="0.00">
                   <c:v>5.9229510000000003</c:v>
                 </c:pt>
-                <c:pt idx="30">
+                <c:pt idx="30" formatCode="0.00">
                   <c:v>5.9229510000000003</c:v>
                 </c:pt>
-                <c:pt idx="31">
+                <c:pt idx="31" formatCode="0.00">
                   <c:v>5.8846999999999996</c:v>
                 </c:pt>
-                <c:pt idx="32">
+                <c:pt idx="32" formatCode="0.00">
                   <c:v>5.8846999999999996</c:v>
                 </c:pt>
-                <c:pt idx="33">
+                <c:pt idx="33" formatCode="0.00">
                   <c:v>5.8846999999999996</c:v>
                 </c:pt>
-                <c:pt idx="34">
+                <c:pt idx="34" formatCode="0.00">
                   <c:v>5.8846999999999996</c:v>
                 </c:pt>
-                <c:pt idx="35">
+                <c:pt idx="35" formatCode="0.00">
                   <c:v>5.6992289999999999</c:v>
                 </c:pt>
-                <c:pt idx="36">
+                <c:pt idx="36" formatCode="0.00">
                   <c:v>4.8929150000000003</c:v>
                 </c:pt>
-                <c:pt idx="37">
+                <c:pt idx="37" formatCode="0.00">
                   <c:v>4.8929150000000003</c:v>
                 </c:pt>
-                <c:pt idx="38">
+                <c:pt idx="38" formatCode="0.00">
                   <c:v>4.8929150000000003</c:v>
                 </c:pt>
-                <c:pt idx="39">
+                <c:pt idx="39" formatCode="0.00">
                   <c:v>4.8929150000000003</c:v>
                 </c:pt>
-                <c:pt idx="40">
+                <c:pt idx="40" formatCode="0.00">
                   <c:v>4.8929150000000003</c:v>
                 </c:pt>
               </c:numCache>
@@ -24875,7 +24874,7 @@
   <dimension ref="A1:P47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="C2" sqref="C2:F42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -24928,9 +24927,12 @@
       <c r="B2">
         <v>0</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="2">
         <v>0</v>
       </c>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
       <c r="G2">
         <v>0</v>
       </c>
@@ -24951,9 +24953,12 @@
       <c r="B3">
         <v>0</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="2">
         <v>0</v>
       </c>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
       <c r="G3">
         <v>0</v>
       </c>
@@ -24974,9 +24979,12 @@
       <c r="B4">
         <v>2</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="2">
         <v>0</v>
       </c>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
       <c r="G4">
         <v>0</v>
       </c>
@@ -24997,16 +25005,16 @@
       <c r="B5">
         <v>0</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="2">
         <v>0.2</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="2">
         <v>5.3073741064902578</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="2">
         <v>5.3790333434146422</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="2">
         <v>5.3826309192012474</v>
       </c>
       <c r="G5">
@@ -25029,16 +25037,16 @@
       <c r="B6">
         <v>10</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="2">
         <v>0.18</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="2">
         <v>5.3073741064902578</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="2">
         <v>5.3790333434146422</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="2">
         <v>5.3826309192012474</v>
       </c>
       <c r="G6">
@@ -25061,16 +25069,16 @@
       <c r="B7">
         <v>52</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="2">
         <v>1.1619999999999999</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="2">
         <v>5.2972558401750414</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="2">
         <v>5.3607218200774787</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="2">
         <v>5.3637747139656771</v>
       </c>
       <c r="G7">
@@ -25093,16 +25101,16 @@
       <c r="B8">
         <v>0</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="2">
         <v>6.2458</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="2">
         <v>6.1360165785574061</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="2">
         <v>6.0616137169026834</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="2">
         <v>6.0645218126048821</v>
       </c>
       <c r="G8">
@@ -25125,16 +25133,16 @@
       <c r="B9">
         <v>0</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="2">
         <v>5.6212200000000001</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="2">
         <v>6.1360165785574061</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="2">
         <v>6.0616137169026834</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="2">
         <v>6.0645218126048821</v>
       </c>
       <c r="G9">
@@ -25157,16 +25165,16 @@
       <c r="B10">
         <v>0</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="2">
         <v>5.0590980000000014</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="2">
         <v>6.1360165785574061</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="2">
         <v>6.0616137169026834</v>
       </c>
-      <c r="F10">
+      <c r="F10" s="2">
         <v>6.0645218126048821</v>
       </c>
       <c r="G10">
@@ -25189,16 +25197,16 @@
       <c r="B11">
         <v>0</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="2">
         <v>4.553188200000001</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="2">
         <v>6.1360165785574061</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="2">
         <v>6.0616137169026834</v>
       </c>
-      <c r="F11">
+      <c r="F11" s="2">
         <v>6.0645218126048821</v>
       </c>
       <c r="G11">
@@ -25221,16 +25229,16 @@
       <c r="B12">
         <v>0</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="2">
         <v>4.0978693800000006</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="2">
         <v>6.1360165785574061</v>
       </c>
-      <c r="E12">
+      <c r="E12" s="2">
         <v>6.0616137169026834</v>
       </c>
-      <c r="F12">
+      <c r="F12" s="2">
         <v>6.0645218126048821</v>
       </c>
       <c r="G12">
@@ -25253,16 +25261,16 @@
       <c r="B13">
         <v>10</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="2">
         <v>3.688082442000002</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="2">
         <v>6.1360165785574061</v>
       </c>
-      <c r="E13">
+      <c r="E13" s="2">
         <v>6.0616137169026834</v>
       </c>
-      <c r="F13">
+      <c r="F13" s="2">
         <v>6.0645218126048821</v>
       </c>
       <c r="G13">
@@ -25285,16 +25293,16 @@
       <c r="B14">
         <v>0</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="2">
         <v>4.3192741978000013</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="2">
         <v>5.6581184576317893</v>
       </c>
-      <c r="E14">
+      <c r="E14" s="2">
         <v>5.6320416104664979</v>
       </c>
-      <c r="F14">
+      <c r="F14" s="2">
         <v>5.6330913563831349</v>
       </c>
       <c r="G14">
@@ -25317,16 +25325,16 @@
       <c r="B15">
         <v>0</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="2">
         <v>3.8873467780200008</v>
       </c>
-      <c r="D15">
+      <c r="D15" s="2">
         <v>5.6581184576317893</v>
       </c>
-      <c r="E15">
+      <c r="E15" s="2">
         <v>5.6320416104664979</v>
       </c>
-      <c r="F15">
+      <c r="F15" s="2">
         <v>5.6330913563831349</v>
       </c>
       <c r="G15">
@@ -25349,16 +25357,16 @@
       <c r="B16">
         <v>0</v>
       </c>
-      <c r="C16">
+      <c r="C16" s="2">
         <v>3.4986121002180011</v>
       </c>
-      <c r="D16">
+      <c r="D16" s="2">
         <v>5.6581184576317893</v>
       </c>
-      <c r="E16">
+      <c r="E16" s="2">
         <v>5.6320416104664979</v>
       </c>
-      <c r="F16">
+      <c r="F16" s="2">
         <v>5.6330913563831349</v>
       </c>
       <c r="G16">
@@ -25381,16 +25389,16 @@
       <c r="B17">
         <v>6</v>
       </c>
-      <c r="C17">
+      <c r="C17" s="2">
         <v>3.1487508901962009</v>
       </c>
-      <c r="D17">
+      <c r="D17" s="2">
         <v>5.6581184576317893</v>
       </c>
-      <c r="E17">
+      <c r="E17" s="2">
         <v>5.6320416104664979</v>
       </c>
-      <c r="F17">
+      <c r="F17" s="2">
         <v>5.6330913563831349</v>
       </c>
       <c r="G17">
@@ -25413,16 +25421,16 @@
       <c r="B18">
         <v>11</v>
       </c>
-      <c r="C18">
+      <c r="C18" s="2">
         <v>3.4338758011765811</v>
       </c>
-      <c r="D18">
+      <c r="D18" s="2">
         <v>5.3529428850624203</v>
       </c>
-      <c r="E18">
+      <c r="E18" s="2">
         <v>5.3529438841633157</v>
       </c>
-      <c r="F18">
+      <c r="F18" s="2">
         <v>5.3529596889218212</v>
       </c>
       <c r="G18">
@@ -25445,16 +25453,16 @@
       <c r="B19">
         <v>0</v>
       </c>
-      <c r="C19">
+      <c r="C19" s="2">
         <v>4.1904882210589234</v>
       </c>
-      <c r="D19">
+      <c r="D19" s="2">
         <v>5.4657685057395211</v>
       </c>
-      <c r="E19">
+      <c r="E19" s="2">
         <v>5.4451725860703277</v>
       </c>
-      <c r="F19">
+      <c r="F19" s="2">
         <v>5.4448906621997306</v>
       </c>
       <c r="G19">
@@ -25477,16 +25485,16 @@
       <c r="B20">
         <v>2</v>
       </c>
-      <c r="C20">
+      <c r="C20" s="2">
         <v>3.7714393989530302</v>
       </c>
-      <c r="D20">
+      <c r="D20" s="2">
         <v>5.4657685057395211</v>
       </c>
-      <c r="E20">
+      <c r="E20" s="2">
         <v>5.4451725860703277</v>
       </c>
-      <c r="F20">
+      <c r="F20" s="2">
         <v>5.4448906621997306</v>
       </c>
       <c r="G20">
@@ -25509,16 +25517,16 @@
       <c r="B21">
         <v>52</v>
       </c>
-      <c r="C21">
+      <c r="C21" s="2">
         <v>3.5942954590577272</v>
       </c>
-      <c r="D21">
+      <c r="D21" s="2">
         <v>5.2759219147797003</v>
       </c>
-      <c r="E21">
+      <c r="E21" s="2">
         <v>5.2714087043514626</v>
       </c>
-      <c r="F21">
+      <c r="F21" s="2">
         <v>5.2706234711538071</v>
       </c>
       <c r="G21">
@@ -25541,16 +25549,16 @@
       <c r="B22">
         <v>18</v>
       </c>
-      <c r="C22">
+      <c r="C22" s="2">
         <v>8.4348659131519543</v>
       </c>
-      <c r="D22">
+      <c r="D22" s="2">
         <v>6.3539675025467419</v>
       </c>
-      <c r="E22">
+      <c r="E22" s="2">
         <v>6.1991626265114244</v>
       </c>
-      <c r="F22">
+      <c r="F22" s="2">
         <v>6.1976650807466216</v>
       </c>
       <c r="G22">
@@ -25573,16 +25581,16 @@
       <c r="B23">
         <v>6</v>
       </c>
-      <c r="C23">
+      <c r="C23" s="2">
         <v>9.3913793218367587</v>
       </c>
-      <c r="D23">
+      <c r="D23" s="2">
         <v>6.6450650369781039</v>
       </c>
-      <c r="E23">
+      <c r="E23" s="2">
         <v>6.4479920356355391</v>
       </c>
-      <c r="F23">
+      <c r="F23" s="2">
         <v>6.446009737727425</v>
       </c>
       <c r="G23">
@@ -25605,16 +25613,16 @@
       <c r="B24">
         <v>3</v>
       </c>
-      <c r="C24">
+      <c r="C24" s="2">
         <v>9.0522413896530836</v>
       </c>
-      <c r="D24">
+      <c r="D24" s="2">
         <v>6.6276339508819868</v>
       </c>
-      <c r="E24">
+      <c r="E24" s="2">
         <v>6.429490034566582</v>
       </c>
-      <c r="F24">
+      <c r="F24" s="2">
         <v>6.4271245044517427</v>
       </c>
       <c r="G24">
@@ -25637,16 +25645,16 @@
       <c r="B25">
         <v>1</v>
       </c>
-      <c r="C25">
+      <c r="C25" s="2">
         <v>8.447017250687777</v>
       </c>
-      <c r="D25">
+      <c r="D25" s="2">
         <v>6.5218903097315541</v>
       </c>
-      <c r="E25">
+      <c r="E25" s="2">
         <v>6.3337430009431896</v>
       </c>
-      <c r="F25">
+      <c r="F25" s="2">
         <v>6.3310230282981843</v>
       </c>
       <c r="G25">
@@ -25669,16 +25677,16 @@
       <c r="B26">
         <v>0</v>
       </c>
-      <c r="C26">
+      <c r="C26" s="2">
         <v>7.7023155256190003</v>
       </c>
-      <c r="D26">
+      <c r="D26" s="2">
         <v>6.348656366815848</v>
       </c>
-      <c r="E26">
+      <c r="E26" s="2">
         <v>6.1783517861701513</v>
       </c>
-      <c r="F26">
+      <c r="F26" s="2">
         <v>6.1753093617476669</v>
       </c>
       <c r="G26">
@@ -25701,16 +25709,16 @@
       <c r="B27">
         <v>4</v>
       </c>
-      <c r="C27">
+      <c r="C27" s="2">
         <v>6.9320839730570993</v>
       </c>
-      <c r="D27">
+      <c r="D27" s="2">
         <v>6.348656366815848</v>
       </c>
-      <c r="E27">
+      <c r="E27" s="2">
         <v>6.1783517861701513</v>
       </c>
-      <c r="F27">
+      <c r="F27" s="2">
         <v>6.1753093617476669</v>
       </c>
       <c r="G27">
@@ -25733,16 +25741,16 @@
       <c r="B28">
         <v>10</v>
       </c>
-      <c r="C28">
+      <c r="C28" s="2">
         <v>6.6388755757513902</v>
       </c>
-      <c r="D28">
+      <c r="D28" s="2">
         <v>6.0652436816714967</v>
       </c>
-      <c r="E28">
+      <c r="E28" s="2">
         <v>5.9204779324111527</v>
       </c>
-      <c r="F28">
+      <c r="F28" s="2">
         <v>5.9167946093454704</v>
       </c>
       <c r="G28">
@@ -25765,16 +25773,16 @@
       <c r="B29">
         <v>0</v>
       </c>
-      <c r="C29">
+      <c r="C29" s="2">
         <v>6.9749880181762514</v>
       </c>
-      <c r="D29">
+      <c r="D29" s="2">
         <v>6.2027311256979303</v>
       </c>
-      <c r="E29">
+      <c r="E29" s="2">
         <v>6.0364568152147342</v>
       </c>
-      <c r="F29">
+      <c r="F29" s="2">
         <v>6.0322593177567692</v>
       </c>
       <c r="G29">
@@ -25797,16 +25805,16 @@
       <c r="B30">
         <v>0</v>
       </c>
-      <c r="C30">
+      <c r="C30" s="2">
         <v>6.2774892163586262</v>
       </c>
-      <c r="D30">
+      <c r="D30" s="2">
         <v>6.2027311256979303</v>
       </c>
-      <c r="E30">
+      <c r="E30" s="2">
         <v>6.0364568152147342</v>
       </c>
-      <c r="F30">
+      <c r="F30" s="2">
         <v>6.0322593177567692</v>
       </c>
       <c r="G30">
@@ -25829,16 +25837,16 @@
       <c r="B31">
         <v>0</v>
       </c>
-      <c r="C31">
+      <c r="C31" s="2">
         <v>5.649740294722764</v>
       </c>
-      <c r="D31">
+      <c r="D31" s="2">
         <v>6.2027311256979303</v>
       </c>
-      <c r="E31">
+      <c r="E31" s="2">
         <v>6.0364568152147342</v>
       </c>
-      <c r="F31">
+      <c r="F31" s="2">
         <v>6.0322593177567692</v>
       </c>
       <c r="G31">
@@ -25861,16 +25869,16 @@
       <c r="B32">
         <v>0</v>
       </c>
-      <c r="C32">
+      <c r="C32" s="2">
         <v>5.0847662652504884</v>
       </c>
-      <c r="D32">
+      <c r="D32" s="2">
         <v>6.2027311256979303</v>
       </c>
-      <c r="E32">
+      <c r="E32" s="2">
         <v>6.0364568152147342</v>
       </c>
-      <c r="F32">
+      <c r="F32" s="2">
         <v>6.0322593177567692</v>
       </c>
       <c r="G32">
@@ -25893,16 +25901,16 @@
       <c r="B33">
         <v>0</v>
       </c>
-      <c r="C33">
+      <c r="C33" s="2">
         <v>4.5762896387254388</v>
       </c>
-      <c r="D33">
+      <c r="D33" s="2">
         <v>6.2027311256979303</v>
       </c>
-      <c r="E33">
+      <c r="E33" s="2">
         <v>6.0364568152147342</v>
       </c>
-      <c r="F33">
+      <c r="F33" s="2">
         <v>6.0322593177567692</v>
       </c>
       <c r="G33">
@@ -25937,16 +25945,16 @@
       <c r="B34">
         <v>0</v>
       </c>
-      <c r="C34">
+      <c r="C34" s="2">
         <v>4.1186606748528947</v>
       </c>
-      <c r="D34">
+      <c r="D34" s="2">
         <v>6.2027311256979303</v>
       </c>
-      <c r="E34">
+      <c r="E34" s="2">
         <v>6.0364568152147342</v>
       </c>
-      <c r="F34">
+      <c r="F34" s="2">
         <v>6.0322593177567692</v>
       </c>
       <c r="G34">
@@ -25984,16 +25992,16 @@
       <c r="B35">
         <v>0</v>
       </c>
-      <c r="C35">
+      <c r="C35" s="2">
         <v>3.7067946073676059</v>
       </c>
-      <c r="D35">
+      <c r="D35" s="2">
         <v>6.2027311256979303</v>
       </c>
-      <c r="E35">
+      <c r="E35" s="2">
         <v>6.0364568152147342</v>
       </c>
-      <c r="F35">
+      <c r="F35" s="2">
         <v>6.0322593177567692</v>
       </c>
       <c r="G35">
@@ -26031,16 +26039,16 @@
       <c r="B36">
         <v>11</v>
       </c>
-      <c r="C36">
+      <c r="C36" s="2">
         <v>3.3361151466308452</v>
       </c>
-      <c r="D36">
+      <c r="D36" s="2">
         <v>6.2027311256979303</v>
       </c>
-      <c r="E36">
+      <c r="E36" s="2">
         <v>6.0364568152147342</v>
       </c>
-      <c r="F36">
+      <c r="F36" s="2">
         <v>6.0322593177567692</v>
       </c>
       <c r="G36">
@@ -26078,16 +26086,16 @@
       <c r="B37">
         <v>3</v>
       </c>
-      <c r="C37">
+      <c r="C37" s="2">
         <v>4.1025036319677604</v>
       </c>
-      <c r="D37">
+      <c r="D37" s="2">
         <v>5.0586214315586426</v>
       </c>
-      <c r="E37">
+      <c r="E37" s="2">
         <v>4.9787540537709774</v>
       </c>
-      <c r="F37">
+      <c r="F37" s="2">
         <v>4.9731254451664082</v>
       </c>
       <c r="G37">
@@ -26123,16 +26131,16 @@
       </c>
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="C38">
+      <c r="C38" s="2">
         <v>3.9922529999999998</v>
       </c>
-      <c r="D38">
+      <c r="D38" s="2">
         <v>4.9930209999999997</v>
       </c>
-      <c r="E38">
+      <c r="E38" s="2">
         <v>4.9146340000000004</v>
       </c>
-      <c r="F38">
+      <c r="F38" s="2">
         <v>4.9088450000000003</v>
       </c>
       <c r="L38" s="11" t="s">
@@ -26144,16 +26152,16 @@
       <c r="P38" s="11"/>
     </row>
     <row r="39" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="C39">
+      <c r="C39" s="2">
         <v>3.9922529999999998</v>
       </c>
-      <c r="D39">
+      <c r="D39" s="2">
         <v>4.9930209999999997</v>
       </c>
-      <c r="E39">
+      <c r="E39" s="2">
         <v>4.9146340000000004</v>
       </c>
-      <c r="F39">
+      <c r="F39" s="2">
         <v>4.9088450000000003</v>
       </c>
       <c r="L39" s="3" t="s">
@@ -26174,16 +26182,16 @@
       </c>
     </row>
     <row r="40" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="C40">
+      <c r="C40" s="2">
         <v>3.9922529999999998</v>
       </c>
-      <c r="D40">
+      <c r="D40" s="2">
         <v>4.9930209999999997</v>
       </c>
-      <c r="E40">
+      <c r="E40" s="2">
         <v>4.9146340000000004</v>
       </c>
-      <c r="F40">
+      <c r="F40" s="2">
         <v>4.9088450000000003</v>
       </c>
       <c r="L40" s="3" t="s">
@@ -26204,16 +26212,16 @@
       </c>
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="C41">
+      <c r="C41" s="2">
         <v>3.9922529999999998</v>
       </c>
-      <c r="D41">
+      <c r="D41" s="2">
         <v>4.9930209999999997</v>
       </c>
-      <c r="E41">
+      <c r="E41" s="2">
         <v>4.9146340000000004</v>
       </c>
-      <c r="F41">
+      <c r="F41" s="2">
         <v>4.9088450000000003</v>
       </c>
       <c r="L41" s="3" t="s">
@@ -26234,16 +26242,16 @@
       </c>
     </row>
     <row r="42" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="C42">
+      <c r="C42" s="2">
         <v>3.9922529999999998</v>
       </c>
-      <c r="D42">
+      <c r="D42" s="2">
         <v>4.9930209999999997</v>
       </c>
-      <c r="E42">
+      <c r="E42" s="2">
         <v>4.9146340000000004</v>
       </c>
-      <c r="F42">
+      <c r="F42" s="2">
         <v>4.9088450000000003</v>
       </c>
       <c r="L42" s="3" t="s">
@@ -26358,8 +26366,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P47"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="Z9" sqref="Z9"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection sqref="A1:F42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -26407,9 +26415,12 @@
       <c r="B2">
         <v>0</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="2">
         <v>0</v>
       </c>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
       <c r="G2">
         <v>0</v>
       </c>
@@ -26430,9 +26441,12 @@
       <c r="B3">
         <v>0</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="2">
         <v>0</v>
       </c>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
       <c r="G3">
         <v>0</v>
       </c>
@@ -26453,9 +26467,12 @@
       <c r="B4">
         <v>2</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="2">
         <v>0</v>
       </c>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
       <c r="G4">
         <v>0</v>
       </c>
@@ -26476,16 +26493,16 @@
       <c r="B5">
         <v>0</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="2">
         <v>0.3</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="2">
         <v>4.8942440594470114</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="2">
         <v>5.1464625281898337</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="2">
         <v>5.1559946109209687</v>
       </c>
       <c r="G5">
@@ -26508,16 +26525,16 @@
       <c r="B6">
         <v>10</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="2">
         <v>0.255</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="2">
         <v>4.8942440594470114</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="2">
         <v>5.1464625281898337</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="2">
         <v>5.1559946109209687</v>
       </c>
       <c r="G6">
@@ -26540,16 +26557,16 @@
       <c r="B7">
         <v>52</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="2">
         <v>1.71675</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="2">
         <v>4.8987126212520868</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="2">
         <v>5.1244288881145099</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="2">
         <v>5.1322734763946087</v>
       </c>
       <c r="G7">
@@ -26572,16 +26589,16 @@
       <c r="B8">
         <v>0</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="2">
         <v>9.2592374999999993</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="2">
         <v>6.0410237856510376</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="2">
         <v>6.1666825870232147</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="2">
         <v>6.1666677218674506</v>
       </c>
       <c r="G8">
@@ -26604,16 +26621,16 @@
       <c r="B9">
         <v>0</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="2">
         <v>7.870351874999999</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="2">
         <v>6.0410237856510376</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="2">
         <v>6.1666825870232147</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="2">
         <v>6.1666677218674506</v>
       </c>
       <c r="G9">
@@ -26636,16 +26653,16 @@
       <c r="B10">
         <v>0</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="2">
         <v>6.6897990937499987</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="2">
         <v>6.0410237856510376</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="2">
         <v>6.1666825870232147</v>
       </c>
-      <c r="F10">
+      <c r="F10" s="2">
         <v>6.1666677218674506</v>
       </c>
       <c r="G10">
@@ -26668,16 +26685,16 @@
       <c r="B11">
         <v>0</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="2">
         <v>5.686329229687499</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="2">
         <v>6.0410237856510376</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="2">
         <v>6.1666825870232147</v>
       </c>
-      <c r="F11">
+      <c r="F11" s="2">
         <v>6.1666677218674506</v>
       </c>
       <c r="G11">
@@ -26700,16 +26717,16 @@
       <c r="B12">
         <v>0</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="2">
         <v>4.8333798452343739</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="2">
         <v>6.0410237856510376</v>
       </c>
-      <c r="E12">
+      <c r="E12" s="2">
         <v>6.1666825870232147</v>
       </c>
-      <c r="F12">
+      <c r="F12" s="2">
         <v>6.1666677218674506</v>
       </c>
       <c r="G12">
@@ -26732,16 +26749,16 @@
       <c r="B13">
         <v>10</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="2">
         <v>4.1083728684492176</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="2">
         <v>6.0410237856510376</v>
       </c>
-      <c r="E13">
+      <c r="E13" s="2">
         <v>6.1666825870232147</v>
       </c>
-      <c r="F13">
+      <c r="F13" s="2">
         <v>6.1666677218674506</v>
       </c>
       <c r="G13">
@@ -26764,16 +26781,16 @@
       <c r="B14">
         <v>0</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="2">
         <v>4.9921169381818347</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="2">
         <v>5.40162761129021</v>
       </c>
-      <c r="E14">
+      <c r="E14" s="2">
         <v>5.4906476304323117</v>
       </c>
-      <c r="F14">
+      <c r="F14" s="2">
         <v>5.4891536355419381</v>
       </c>
       <c r="G14">
@@ -26796,16 +26813,16 @@
       <c r="B15">
         <v>0</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="2">
         <v>4.2432993974545594</v>
       </c>
-      <c r="D15">
+      <c r="D15" s="2">
         <v>5.40162761129021</v>
       </c>
-      <c r="E15">
+      <c r="E15" s="2">
         <v>5.4906476304323117</v>
       </c>
-      <c r="F15">
+      <c r="F15" s="2">
         <v>5.4891536355419381</v>
       </c>
       <c r="G15">
@@ -26828,16 +26845,16 @@
       <c r="B16">
         <v>0</v>
       </c>
-      <c r="C16">
+      <c r="C16" s="2">
         <v>3.6068044878363752</v>
       </c>
-      <c r="D16">
+      <c r="D16" s="2">
         <v>5.40162761129021</v>
       </c>
-      <c r="E16">
+      <c r="E16" s="2">
         <v>5.4906476304323117</v>
       </c>
-      <c r="F16">
+      <c r="F16" s="2">
         <v>5.4891536355419381</v>
       </c>
       <c r="G16">
@@ -26860,16 +26877,16 @@
       <c r="B17">
         <v>6</v>
       </c>
-      <c r="C17">
+      <c r="C17" s="2">
         <v>3.0657838146609189</v>
       </c>
-      <c r="D17">
+      <c r="D17" s="2">
         <v>5.40162761129021</v>
       </c>
-      <c r="E17">
+      <c r="E17" s="2">
         <v>5.4906476304323117</v>
       </c>
-      <c r="F17">
+      <c r="F17" s="2">
         <v>5.4891536355419381</v>
       </c>
       <c r="G17">
@@ -26892,16 +26909,16 @@
       <c r="B18">
         <v>11</v>
       </c>
-      <c r="C18">
+      <c r="C18" s="2">
         <v>3.5059162424617809</v>
       </c>
-      <c r="D18">
+      <c r="D18" s="2">
         <v>5.0003399239190527</v>
       </c>
-      <c r="E18">
+      <c r="E18" s="2">
         <v>5.0686332285457114</v>
       </c>
-      <c r="F18">
+      <c r="F18" s="2">
         <v>5.0663548013247741</v>
       </c>
       <c r="G18">
@@ -26924,16 +26941,16 @@
       <c r="B19">
         <v>0</v>
       </c>
-      <c r="C19">
+      <c r="C19" s="2">
         <v>4.630028806092513</v>
       </c>
-      <c r="D19">
+      <c r="D19" s="2">
         <v>5.1765030285121343</v>
       </c>
-      <c r="E19">
+      <c r="E19" s="2">
         <v>5.2185673305684732</v>
       </c>
-      <c r="F19">
+      <c r="F19" s="2">
         <v>5.214391683581642</v>
       </c>
       <c r="G19">
@@ -26956,16 +26973,16 @@
       <c r="B20">
         <v>2</v>
       </c>
-      <c r="C20">
+      <c r="C20" s="2">
         <v>3.935524485178636</v>
       </c>
-      <c r="D20">
+      <c r="D20" s="2">
         <v>5.1765030285121343</v>
       </c>
-      <c r="E20">
+      <c r="E20" s="2">
         <v>5.2185673305684732</v>
       </c>
-      <c r="F20">
+      <c r="F20" s="2">
         <v>5.214391683581642</v>
       </c>
       <c r="G20">
@@ -26988,16 +27005,16 @@
       <c r="B21">
         <v>52</v>
       </c>
-      <c r="C21">
+      <c r="C21" s="2">
         <v>3.6451958124018402</v>
       </c>
-      <c r="D21">
+      <c r="D21" s="2">
         <v>4.9066054827365964</v>
       </c>
-      <c r="E21">
+      <c r="E21" s="2">
         <v>4.9411046913473093</v>
       </c>
-      <c r="F21">
+      <c r="F21" s="2">
         <v>4.9368059572001304</v>
       </c>
       <c r="G21">
@@ -27020,16 +27037,16 @@
       <c r="B22">
         <v>18</v>
       </c>
-      <c r="C22">
+      <c r="C22" s="2">
         <v>10.89841644054156</v>
       </c>
-      <c r="D22">
+      <c r="D22" s="2">
         <v>6.6312287102875329</v>
       </c>
-      <c r="E22">
+      <c r="E22" s="2">
         <v>6.521641636345727</v>
       </c>
-      <c r="F22">
+      <c r="F22" s="2">
         <v>6.5059198049515636</v>
       </c>
       <c r="G22">
@@ -27052,16 +27069,16 @@
       <c r="B23">
         <v>6</v>
       </c>
-      <c r="C23">
+      <c r="C23" s="2">
         <v>11.96365397446033</v>
       </c>
-      <c r="D23">
+      <c r="D23" s="2">
         <v>7.1008087029099149</v>
       </c>
-      <c r="E23">
+      <c r="E23" s="2">
         <v>6.9399872376291674</v>
       </c>
-      <c r="F23">
+      <c r="F23" s="2">
         <v>6.92039356582137</v>
       </c>
       <c r="G23">
@@ -27084,16 +27101,16 @@
       <c r="B24">
         <v>3</v>
       </c>
-      <c r="C24">
+      <c r="C24" s="2">
         <v>11.06910587829128</v>
       </c>
-      <c r="D24">
+      <c r="D24" s="2">
         <v>7.0497955846733174</v>
       </c>
-      <c r="E24">
+      <c r="E24" s="2">
         <v>6.8755731413838008</v>
       </c>
-      <c r="F24">
+      <c r="F24" s="2">
         <v>6.8551966409897016</v>
       </c>
       <c r="G24">
@@ -27116,16 +27133,16 @@
       <c r="B25">
         <v>1</v>
       </c>
-      <c r="C25">
+      <c r="C25" s="2">
         <v>9.8587399965475857</v>
       </c>
-      <c r="D25">
+      <c r="D25" s="2">
         <v>6.8404182734165868</v>
       </c>
-      <c r="E25">
+      <c r="E25" s="2">
         <v>6.663570553409599</v>
       </c>
-      <c r="F25">
+      <c r="F25" s="2">
         <v>6.6433043742062416</v>
       </c>
       <c r="G25">
@@ -27148,16 +27165,16 @@
       <c r="B26">
         <v>0</v>
       </c>
-      <c r="C26">
+      <c r="C26" s="2">
         <v>8.5299289970654488</v>
       </c>
-      <c r="D26">
+      <c r="D26" s="2">
         <v>6.5055468756693724</v>
       </c>
-      <c r="E26">
+      <c r="E26" s="2">
         <v>6.3345387269079474</v>
       </c>
-      <c r="F26">
+      <c r="F26" s="2">
         <v>6.3150859213908408</v>
       </c>
       <c r="G26">
@@ -27180,16 +27197,16 @@
       <c r="B27">
         <v>4</v>
       </c>
-      <c r="C27">
+      <c r="C27" s="2">
         <v>7.2504396475056314</v>
       </c>
-      <c r="D27">
+      <c r="D27" s="2">
         <v>6.5055468756693724</v>
       </c>
-      <c r="E27">
+      <c r="E27" s="2">
         <v>6.3345387269079474</v>
       </c>
-      <c r="F27">
+      <c r="F27" s="2">
         <v>6.3150859213908408</v>
       </c>
       <c r="G27">
@@ -27212,16 +27229,16 @@
       <c r="B28">
         <v>10</v>
       </c>
-      <c r="C28">
+      <c r="C28" s="2">
         <v>6.7628737003797861</v>
       </c>
-      <c r="D28">
+      <c r="D28" s="2">
         <v>5.9699585021403081</v>
       </c>
-      <c r="E28">
+      <c r="E28" s="2">
         <v>5.8014475718881533</v>
       </c>
-      <c r="F28">
+      <c r="F28" s="2">
         <v>5.7828614910931053</v>
       </c>
       <c r="G28">
@@ -27244,16 +27261,16 @@
       <c r="B29">
         <v>0</v>
       </c>
-      <c r="C29">
+      <c r="C29" s="2">
         <v>7.2484426453228181</v>
       </c>
-      <c r="D29">
+      <c r="D29" s="2">
         <v>6.2333433238355704</v>
       </c>
-      <c r="E29">
+      <c r="E29" s="2">
         <v>6.0268289986069963</v>
       </c>
-      <c r="F29">
+      <c r="F29" s="2">
         <v>6.0054832801958424</v>
       </c>
       <c r="G29">
@@ -27276,16 +27293,16 @@
       <c r="B30">
         <v>0</v>
       </c>
-      <c r="C30">
+      <c r="C30" s="2">
         <v>6.161176248524395</v>
       </c>
-      <c r="D30">
+      <c r="D30" s="2">
         <v>6.2333433238355704</v>
       </c>
-      <c r="E30">
+      <c r="E30" s="2">
         <v>6.0268289986069963</v>
       </c>
-      <c r="F30">
+      <c r="F30" s="2">
         <v>6.0054832801958424</v>
       </c>
       <c r="G30">
@@ -27308,16 +27325,16 @@
       <c r="B31">
         <v>0</v>
       </c>
-      <c r="C31">
+      <c r="C31" s="2">
         <v>5.2369998112457354</v>
       </c>
-      <c r="D31">
+      <c r="D31" s="2">
         <v>6.2333433238355704</v>
       </c>
-      <c r="E31">
+      <c r="E31" s="2">
         <v>6.0268289986069963</v>
       </c>
-      <c r="F31">
+      <c r="F31" s="2">
         <v>6.0054832801958424</v>
       </c>
       <c r="G31">
@@ -27340,16 +27357,16 @@
       <c r="B32">
         <v>0</v>
       </c>
-      <c r="C32">
+      <c r="C32" s="2">
         <v>4.4514498395588751</v>
       </c>
-      <c r="D32">
+      <c r="D32" s="2">
         <v>6.2333433238355704</v>
       </c>
-      <c r="E32">
+      <c r="E32" s="2">
         <v>6.0268289986069963</v>
       </c>
-      <c r="F32">
+      <c r="F32" s="2">
         <v>6.0054832801958424</v>
       </c>
       <c r="G32">
@@ -27372,16 +27389,16 @@
       <c r="B33">
         <v>0</v>
       </c>
-      <c r="C33">
+      <c r="C33" s="2">
         <v>3.7837323636250439</v>
       </c>
-      <c r="D33">
+      <c r="D33" s="2">
         <v>6.2333433238355704</v>
       </c>
-      <c r="E33">
+      <c r="E33" s="2">
         <v>6.0268289986069963</v>
       </c>
-      <c r="F33">
+      <c r="F33" s="2">
         <v>6.0054832801958424</v>
       </c>
       <c r="G33">
@@ -27416,16 +27433,16 @@
       <c r="B34">
         <v>0</v>
       </c>
-      <c r="C34">
+      <c r="C34" s="2">
         <v>3.2161725090812872</v>
       </c>
-      <c r="D34">
+      <c r="D34" s="2">
         <v>6.2333433238355704</v>
       </c>
-      <c r="E34">
+      <c r="E34" s="2">
         <v>6.0268289986069963</v>
       </c>
-      <c r="F34">
+      <c r="F34" s="2">
         <v>6.0054832801958424</v>
       </c>
       <c r="G34">
@@ -27463,16 +27480,16 @@
       <c r="B35">
         <v>0</v>
       </c>
-      <c r="C35">
+      <c r="C35" s="2">
         <v>2.733746632719094</v>
       </c>
-      <c r="D35">
+      <c r="D35" s="2">
         <v>6.2333433238355704</v>
       </c>
-      <c r="E35">
+      <c r="E35" s="2">
         <v>6.0268289986069963</v>
       </c>
-      <c r="F35">
+      <c r="F35" s="2">
         <v>6.0054832801958424</v>
       </c>
       <c r="G35">
@@ -27510,16 +27527,16 @@
       <c r="B36">
         <v>11</v>
       </c>
-      <c r="C36">
+      <c r="C36" s="2">
         <v>2.3236846378112301</v>
       </c>
-      <c r="D36">
+      <c r="D36" s="2">
         <v>6.2333433238355704</v>
       </c>
-      <c r="E36">
+      <c r="E36" s="2">
         <v>6.0268289986069963</v>
       </c>
-      <c r="F36">
+      <c r="F36" s="2">
         <v>6.0054832801958424</v>
       </c>
       <c r="G36">
@@ -27557,16 +27574,16 @@
       <c r="B37">
         <v>3</v>
       </c>
-      <c r="C37">
+      <c r="C37" s="2">
         <v>3.6251319421395451</v>
       </c>
-      <c r="D37">
+      <c r="D37" s="2">
         <v>4.3830585571354543</v>
       </c>
-      <c r="E37">
+      <c r="E37" s="2">
         <v>4.2159195630217274</v>
       </c>
-      <c r="F37">
+      <c r="F37" s="2">
         <v>4.1995189728968692</v>
       </c>
       <c r="G37">
@@ -27602,16 +27619,16 @@
       </c>
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="C38">
+      <c r="C38" s="2">
         <v>3.5313620000000001</v>
       </c>
-      <c r="D38">
+      <c r="D38" s="2">
         <v>4.3097060000000003</v>
       </c>
-      <c r="E38">
+      <c r="E38" s="2">
         <v>4.1394979999999997</v>
       </c>
-      <c r="F38">
+      <c r="F38" s="2">
         <v>4.1230000000000002</v>
       </c>
       <c r="L38" s="11" t="s">
@@ -27623,16 +27640,16 @@
       <c r="P38" s="11"/>
     </row>
     <row r="39" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="C39">
+      <c r="C39" s="2">
         <v>3.5313620000000001</v>
       </c>
-      <c r="D39">
+      <c r="D39" s="2">
         <v>4.3097060000000003</v>
       </c>
-      <c r="E39">
+      <c r="E39" s="2">
         <v>4.1394979999999997</v>
       </c>
-      <c r="F39">
+      <c r="F39" s="2">
         <v>4.1230000000000002</v>
       </c>
       <c r="L39" s="3" t="s">
@@ -27653,16 +27670,16 @@
       </c>
     </row>
     <row r="40" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="C40">
+      <c r="C40" s="2">
         <v>3.5313620000000001</v>
       </c>
-      <c r="D40">
+      <c r="D40" s="2">
         <v>4.3097060000000003</v>
       </c>
-      <c r="E40">
+      <c r="E40" s="2">
         <v>4.1394979999999997</v>
       </c>
-      <c r="F40">
+      <c r="F40" s="2">
         <v>4.1230000000000002</v>
       </c>
       <c r="L40" s="3" t="s">
@@ -27683,16 +27700,16 @@
       </c>
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="C41">
+      <c r="C41" s="2">
         <v>3.5313620000000001</v>
       </c>
-      <c r="D41">
+      <c r="D41" s="2">
         <v>4.3097060000000003</v>
       </c>
-      <c r="E41">
+      <c r="E41" s="2">
         <v>4.1394979999999997</v>
       </c>
-      <c r="F41">
+      <c r="F41" s="2">
         <v>4.1230000000000002</v>
       </c>
       <c r="L41" s="3" t="s">
@@ -27713,16 +27730,16 @@
       </c>
     </row>
     <row r="42" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="C42">
+      <c r="C42" s="2">
         <v>3.5313620000000001</v>
       </c>
-      <c r="D42">
+      <c r="D42" s="2">
         <v>4.3097060000000003</v>
       </c>
-      <c r="E42">
+      <c r="E42" s="2">
         <v>4.1394979999999997</v>
       </c>
-      <c r="F42">
+      <c r="F42" s="2">
         <v>4.1230000000000002</v>
       </c>
       <c r="L42" s="3" t="s">
@@ -27837,8 +27854,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P47"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O48" sqref="O48"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection sqref="A1:F42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -27905,9 +27922,12 @@
       <c r="B3">
         <v>0</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="2">
         <v>0</v>
       </c>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
       <c r="G3">
         <v>0</v>
       </c>
@@ -27928,9 +27948,12 @@
       <c r="B4">
         <v>2</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="2">
         <v>0</v>
       </c>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
       <c r="G4">
         <v>0</v>
       </c>
@@ -27951,16 +27974,16 @@
       <c r="B5">
         <v>0</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="2">
         <v>1</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="2">
         <v>3.4673832482421782E-5</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="2">
         <v>1.5681488620568459E-4</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="2">
         <v>1.3939100996060861E-4</v>
       </c>
       <c r="G5">
@@ -27983,16 +28006,16 @@
       <c r="B6">
         <v>10</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="2">
         <v>0.5</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="2">
         <v>3.4673832482421782E-5</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="2">
         <v>1.5681488620568459E-4</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="2">
         <v>1.3939100996060861E-4</v>
       </c>
       <c r="G6">
@@ -28015,16 +28038,16 @@
       <c r="B7">
         <v>52</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="2">
         <v>5.25</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="2">
         <v>1.000027871198983</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="2">
         <v>0.75012559874049023</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="2">
         <v>0.66677830999154697</v>
       </c>
       <c r="G7">
@@ -28047,16 +28070,16 @@
       <c r="B8">
         <v>0</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="2">
         <v>28.625</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="2">
         <v>9.5000241619471719</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="2">
         <v>7.1251057057137617</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="2">
         <v>6.3334272939677883</v>
       </c>
       <c r="G8">
@@ -28079,16 +28102,16 @@
       <c r="B9">
         <v>0</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="2">
         <v>14.3125</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="2">
         <v>9.5000241619471719</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="2">
         <v>7.1251057057137617</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="2">
         <v>6.3334272939677883</v>
       </c>
       <c r="G9">
@@ -28111,16 +28134,16 @@
       <c r="B10">
         <v>0</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="2">
         <v>7.15625</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="2">
         <v>9.5000241619471719</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="2">
         <v>7.1251057057137617</v>
       </c>
-      <c r="F10">
+      <c r="F10" s="2">
         <v>6.3334272939677883</v>
       </c>
       <c r="G10">
@@ -28143,16 +28166,16 @@
       <c r="B11">
         <v>0</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="2">
         <v>3.578125</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="2">
         <v>9.5000241619471719</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="2">
         <v>7.1251057057137617</v>
       </c>
-      <c r="F11">
+      <c r="F11" s="2">
         <v>6.3334272939677883</v>
       </c>
       <c r="G11">
@@ -28175,16 +28198,16 @@
       <c r="B12">
         <v>0</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="2">
         <v>1.7890625</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="2">
         <v>9.5000241619471719</v>
       </c>
-      <c r="E12">
+      <c r="E12" s="2">
         <v>7.1251057057137617</v>
       </c>
-      <c r="F12">
+      <c r="F12" s="2">
         <v>6.3334272939677883</v>
       </c>
       <c r="G12">
@@ -28207,16 +28230,16 @@
       <c r="B13">
         <v>10</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="2">
         <v>0.89453125</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="2">
         <v>9.5000241619471719</v>
       </c>
-      <c r="E13">
+      <c r="E13" s="2">
         <v>7.1251057057137617</v>
       </c>
-      <c r="F13">
+      <c r="F13" s="2">
         <v>6.3334272939677883</v>
       </c>
       <c r="G13">
@@ -28239,16 +28262,16 @@
       <c r="B14">
         <v>0</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="2">
         <v>5.447265625</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="2">
         <v>4.2777856400838568</v>
       </c>
-      <c r="E14">
+      <c r="E14" s="2">
         <v>3.2083683555621949</v>
       </c>
-      <c r="F14">
+      <c r="F14" s="2">
         <v>2.8518829827219512</v>
       </c>
       <c r="G14">
@@ -28271,16 +28294,16 @@
       <c r="B15">
         <v>0</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="2">
         <v>2.7236328125</v>
       </c>
-      <c r="D15">
+      <c r="D15" s="2">
         <v>4.2777856400838568</v>
       </c>
-      <c r="E15">
+      <c r="E15" s="2">
         <v>3.2083683555621949</v>
       </c>
-      <c r="F15">
+      <c r="F15" s="2">
         <v>2.8518829827219512</v>
       </c>
       <c r="G15">
@@ -28303,16 +28326,16 @@
       <c r="B16">
         <v>0</v>
       </c>
-      <c r="C16">
+      <c r="C16" s="2">
         <v>1.36181640625</v>
       </c>
-      <c r="D16">
+      <c r="D16" s="2">
         <v>4.2777856400838568</v>
       </c>
-      <c r="E16">
+      <c r="E16" s="2">
         <v>3.2083683555621949</v>
       </c>
-      <c r="F16">
+      <c r="F16" s="2">
         <v>2.8518829827219512</v>
       </c>
       <c r="G16">
@@ -28335,16 +28358,16 @@
       <c r="B17">
         <v>6</v>
       </c>
-      <c r="C17">
+      <c r="C17" s="2">
         <v>0.680908203125</v>
       </c>
-      <c r="D17">
+      <c r="D17" s="2">
         <v>4.2777856400838568</v>
       </c>
-      <c r="E17">
+      <c r="E17" s="2">
         <v>3.2083683555621949</v>
       </c>
-      <c r="F17">
+      <c r="F17" s="2">
         <v>2.8518829827219512</v>
       </c>
       <c r="G17">
@@ -28367,16 +28390,16 @@
       <c r="B18">
         <v>11</v>
       </c>
-      <c r="C18">
+      <c r="C18" s="2">
         <v>3.3404541015625</v>
       </c>
-      <c r="D18">
+      <c r="D18" s="2">
         <v>2.9705923722907861</v>
       </c>
-      <c r="E18">
+      <c r="E18" s="2">
         <v>2.2279596894229479</v>
       </c>
-      <c r="F18">
+      <c r="F18" s="2">
         <v>1.9804086128203979</v>
       </c>
       <c r="G18">
@@ -28399,16 +28422,16 @@
       <c r="B19">
         <v>0</v>
       </c>
-      <c r="C19">
+      <c r="C19" s="2">
         <v>7.17022705078125</v>
       </c>
-      <c r="D19">
+      <c r="D19" s="2">
         <v>4.5000033730552831</v>
       </c>
-      <c r="E19">
+      <c r="E19" s="2">
         <v>3.3750150134107821</v>
       </c>
-      <c r="F19">
+      <c r="F19" s="2">
         <v>3.000013345254029</v>
       </c>
       <c r="G19">
@@ -28431,16 +28454,16 @@
       <c r="B20">
         <v>2</v>
       </c>
-      <c r="C20">
+      <c r="C20" s="2">
         <v>3.585113525390625</v>
       </c>
-      <c r="D20">
+      <c r="D20" s="2">
         <v>4.5000033730552831</v>
       </c>
-      <c r="E20">
+      <c r="E20" s="2">
         <v>3.3750150134107821</v>
       </c>
-      <c r="F20">
+      <c r="F20" s="2">
         <v>3.000013345254029</v>
       </c>
       <c r="G20">
@@ -28463,16 +28486,16 @@
       <c r="B21">
         <v>52</v>
       </c>
-      <c r="C21">
+      <c r="C21" s="2">
         <v>2.7925567626953129</v>
       </c>
-      <c r="D21">
+      <c r="D21" s="2">
         <v>2.9864883874106591</v>
       </c>
-      <c r="E21">
+      <c r="E21" s="2">
         <v>2.2398733709735499</v>
       </c>
-      <c r="F21">
+      <c r="F21" s="2">
         <v>1.9909985519764899</v>
       </c>
       <c r="G21">
@@ -28495,16 +28518,16 @@
       <c r="B22">
         <v>18</v>
       </c>
-      <c r="C22">
+      <c r="C22" s="2">
         <v>27.39627838134766</v>
       </c>
-      <c r="D22">
+      <c r="D22" s="2">
         <v>17.783020287207599</v>
       </c>
-      <c r="E22">
+      <c r="E22" s="2">
         <v>13.33727019165547</v>
       </c>
-      <c r="F22">
+      <c r="F22" s="2">
         <v>11.855351281471529</v>
       </c>
       <c r="G22">
@@ -28527,16 +28550,16 @@
       <c r="B23">
         <v>6</v>
       </c>
-      <c r="C23">
+      <c r="C23" s="2">
         <v>22.698139190673832</v>
       </c>
-      <c r="D23">
+      <c r="D23" s="2">
         <v>17.864706767635141</v>
       </c>
-      <c r="E23">
+      <c r="E23" s="2">
         <v>13.39853317867912</v>
       </c>
-      <c r="F23">
+      <c r="F23" s="2">
         <v>11.909807269937</v>
       </c>
       <c r="G23">
@@ -28559,16 +28582,16 @@
       <c r="B24">
         <v>3</v>
       </c>
-      <c r="C24">
+      <c r="C24" s="2">
         <v>14.349069595336911</v>
       </c>
-      <c r="D24">
+      <c r="D24" s="2">
         <v>12.76845686956724</v>
       </c>
-      <c r="E24">
+      <c r="E24" s="2">
         <v>9.576344418234374</v>
       </c>
-      <c r="F24">
+      <c r="F24" s="2">
         <v>8.512306149541665</v>
       </c>
       <c r="G24">
@@ -28591,16 +28614,16 @@
       <c r="B25">
         <v>1</v>
       </c>
-      <c r="C25">
+      <c r="C25" s="2">
         <v>8.674534797668457</v>
       </c>
-      <c r="D25">
+      <c r="D25" s="2">
         <v>8.2545128955754716</v>
       </c>
-      <c r="E25">
+      <c r="E25" s="2">
         <v>6.1908856197107536</v>
       </c>
-      <c r="F25">
+      <c r="F25" s="2">
         <v>5.5030094397428924</v>
       </c>
       <c r="G25">
@@ -28623,16 +28646,16 @@
       <c r="B26">
         <v>0</v>
       </c>
-      <c r="C26">
+      <c r="C26" s="2">
         <v>4.8372673988342294</v>
       </c>
-      <c r="D26">
+      <c r="D26" s="2">
         <v>4.7701689885992611</v>
       </c>
-      <c r="E26">
+      <c r="E26" s="2">
         <v>3.577627233359844</v>
       </c>
-      <c r="F26">
+      <c r="F26" s="2">
         <v>3.1801130963198609</v>
       </c>
       <c r="G26">
@@ -28655,16 +28678,16 @@
       <c r="B27">
         <v>4</v>
       </c>
-      <c r="C27">
+      <c r="C27" s="2">
         <v>2.4186336994171138</v>
       </c>
-      <c r="D27">
+      <c r="D27" s="2">
         <v>4.7701689885992611</v>
       </c>
-      <c r="E27">
+      <c r="E27" s="2">
         <v>3.577627233359844</v>
       </c>
-      <c r="F27">
+      <c r="F27" s="2">
         <v>3.1801130963198609</v>
       </c>
       <c r="G27">
@@ -28687,16 +28710,16 @@
       <c r="B28">
         <v>10</v>
       </c>
-      <c r="C28">
+      <c r="C28" s="2">
         <v>3.2093168497085571</v>
       </c>
-      <c r="D28">
+      <c r="D28" s="2">
         <v>2.9482980541564419</v>
       </c>
-      <c r="E28">
+      <c r="E28" s="2">
         <v>2.211223708870905</v>
       </c>
-      <c r="F28">
+      <c r="F28" s="2">
         <v>1.9655321856630259</v>
       </c>
       <c r="G28">
@@ -28719,16 +28742,16 @@
       <c r="B29">
         <v>0</v>
       </c>
-      <c r="C29">
+      <c r="C29" s="2">
         <v>6.6046584248542786</v>
       </c>
-      <c r="D29">
+      <c r="D29" s="2">
         <v>5.7460286986616689</v>
       </c>
-      <c r="E29">
+      <c r="E29" s="2">
         <v>4.3095216256253499</v>
       </c>
-      <c r="F29">
+      <c r="F29" s="2">
         <v>3.830685889444756</v>
       </c>
       <c r="G29">
@@ -28751,16 +28774,16 @@
       <c r="B30">
         <v>0</v>
       </c>
-      <c r="C30">
+      <c r="C30" s="2">
         <v>3.3023292124271388</v>
       </c>
-      <c r="D30">
+      <c r="D30" s="2">
         <v>5.7460286986616689</v>
       </c>
-      <c r="E30">
+      <c r="E30" s="2">
         <v>4.3095216256253499</v>
       </c>
-      <c r="F30">
+      <c r="F30" s="2">
         <v>3.830685889444756</v>
       </c>
       <c r="G30">
@@ -28783,16 +28806,16 @@
       <c r="B31">
         <v>0</v>
       </c>
-      <c r="C31">
+      <c r="C31" s="2">
         <v>1.6511646062135701</v>
       </c>
-      <c r="D31">
+      <c r="D31" s="2">
         <v>5.7460286986616689</v>
       </c>
-      <c r="E31">
+      <c r="E31" s="2">
         <v>4.3095216256253499</v>
       </c>
-      <c r="F31">
+      <c r="F31" s="2">
         <v>3.830685889444756</v>
       </c>
       <c r="G31">
@@ -28815,16 +28838,16 @@
       <c r="B32">
         <v>0</v>
       </c>
-      <c r="C32">
+      <c r="C32" s="2">
         <v>0.82558230310678482</v>
       </c>
-      <c r="D32">
+      <c r="D32" s="2">
         <v>5.7460286986616689</v>
       </c>
-      <c r="E32">
+      <c r="E32" s="2">
         <v>4.3095216256253499</v>
       </c>
-      <c r="F32">
+      <c r="F32" s="2">
         <v>3.830685889444756</v>
       </c>
       <c r="G32">
@@ -28847,16 +28870,16 @@
       <c r="B33">
         <v>0</v>
       </c>
-      <c r="C33">
+      <c r="C33" s="2">
         <v>0.41279115155339241</v>
       </c>
-      <c r="D33">
+      <c r="D33" s="2">
         <v>5.7460286986616689</v>
       </c>
-      <c r="E33">
+      <c r="E33" s="2">
         <v>4.3095216256253499</v>
       </c>
-      <c r="F33">
+      <c r="F33" s="2">
         <v>3.830685889444756</v>
       </c>
       <c r="G33">
@@ -28891,16 +28914,16 @@
       <c r="B34">
         <v>0</v>
       </c>
-      <c r="C34">
+      <c r="C34" s="2">
         <v>0.20639557577669621</v>
       </c>
-      <c r="D34">
+      <c r="D34" s="2">
         <v>5.7460286986616689</v>
       </c>
-      <c r="E34">
+      <c r="E34" s="2">
         <v>4.3095216256253499</v>
       </c>
-      <c r="F34">
+      <c r="F34" s="2">
         <v>3.830685889444756</v>
       </c>
       <c r="G34">
@@ -28938,16 +28961,16 @@
       <c r="B35">
         <v>0</v>
       </c>
-      <c r="C35">
+      <c r="C35" s="2">
         <v>0.1031977878883481</v>
       </c>
-      <c r="D35">
+      <c r="D35" s="2">
         <v>5.7460286986616689</v>
       </c>
-      <c r="E35">
+      <c r="E35" s="2">
         <v>4.3095216256253499</v>
       </c>
-      <c r="F35">
+      <c r="F35" s="2">
         <v>3.830685889444756</v>
       </c>
       <c r="G35">
@@ -28985,16 +29008,16 @@
       <c r="B36">
         <v>11</v>
       </c>
-      <c r="C36">
+      <c r="C36" s="2">
         <v>5.1598893944174051E-2</v>
       </c>
-      <c r="D36">
+      <c r="D36" s="2">
         <v>5.7460286986616689</v>
       </c>
-      <c r="E36">
+      <c r="E36" s="2">
         <v>4.3095216256253499</v>
       </c>
-      <c r="F36">
+      <c r="F36" s="2">
         <v>3.830685889444756</v>
       </c>
       <c r="G36">
@@ -29032,16 +29055,16 @@
       <c r="B37">
         <v>3</v>
       </c>
-      <c r="C37">
+      <c r="C37" s="2">
         <v>5.525799446972087</v>
       </c>
-      <c r="D37">
+      <c r="D37" s="2">
         <v>1.9698655454784271</v>
       </c>
-      <c r="E37">
+      <c r="E37" s="2">
         <v>1.4773991729160469</v>
       </c>
-      <c r="F37">
+      <c r="F37" s="2">
         <v>1.3132437092587079</v>
       </c>
       <c r="G37">
@@ -29077,16 +29100,16 @@
       </c>
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="C38">
+      <c r="C38" s="2">
         <v>4.2629000000000001</v>
       </c>
-      <c r="D38">
+      <c r="D38" s="2">
         <v>2.1528339999999999</v>
       </c>
-      <c r="E38">
+      <c r="E38" s="2">
         <v>1.614625</v>
       </c>
-      <c r="F38">
+      <c r="F38" s="2">
         <v>1.4352229999999999</v>
       </c>
       <c r="L38" s="11" t="s">
@@ -29098,16 +29121,16 @@
       <c r="P38" s="11"/>
     </row>
     <row r="39" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="C39">
+      <c r="C39" s="2">
         <v>4.2629000000000001</v>
       </c>
-      <c r="D39">
+      <c r="D39" s="2">
         <v>2.1528339999999999</v>
       </c>
-      <c r="E39">
+      <c r="E39" s="2">
         <v>1.614625</v>
       </c>
-      <c r="F39">
+      <c r="F39" s="2">
         <v>1.4352229999999999</v>
       </c>
       <c r="L39" s="3" t="s">
@@ -29128,16 +29151,16 @@
       </c>
     </row>
     <row r="40" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="C40">
+      <c r="C40" s="2">
         <v>4.2629000000000001</v>
       </c>
-      <c r="D40">
+      <c r="D40" s="2">
         <v>2.1528339999999999</v>
       </c>
-      <c r="E40">
+      <c r="E40" s="2">
         <v>1.614625</v>
       </c>
-      <c r="F40">
+      <c r="F40" s="2">
         <v>1.4352229999999999</v>
       </c>
       <c r="L40" s="3" t="s">
@@ -29158,16 +29181,16 @@
       </c>
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="C41">
+      <c r="C41" s="2">
         <v>4.2629000000000001</v>
       </c>
-      <c r="D41">
+      <c r="D41" s="2">
         <v>2.1528339999999999</v>
       </c>
-      <c r="E41">
+      <c r="E41" s="2">
         <v>1.614625</v>
       </c>
-      <c r="F41">
+      <c r="F41" s="2">
         <v>1.4352229999999999</v>
       </c>
       <c r="L41" s="3" t="s">
@@ -29188,16 +29211,16 @@
       </c>
     </row>
     <row r="42" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="C42">
+      <c r="C42" s="2">
         <v>4.2629000000000001</v>
       </c>
-      <c r="D42">
+      <c r="D42" s="2">
         <v>2.1528339999999999</v>
       </c>
-      <c r="E42">
+      <c r="E42" s="2">
         <v>1.614625</v>
       </c>
-      <c r="F42">
+      <c r="F42" s="2">
         <v>1.4352229999999999</v>
       </c>
       <c r="L42" s="3" t="s">
@@ -29312,11 +29335,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V56"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="X6" sqref="X6"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection sqref="A1:F42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -29354,12 +29382,15 @@
       <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="2">
         <v>0</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="2">
         <v>0</v>
       </c>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
       <c r="G2">
         <v>0</v>
       </c>
@@ -29377,12 +29408,15 @@
       <c r="A3" t="s">
         <v>3</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="2">
         <v>0</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="2">
         <v>0</v>
       </c>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
       <c r="G3">
         <v>0</v>
       </c>
@@ -29400,12 +29434,15 @@
       <c r="A4" t="s">
         <v>4</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="2">
         <v>2</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="2">
         <v>0</v>
       </c>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
       <c r="G4">
         <v>0</v>
       </c>
@@ -29423,19 +29460,19 @@
       <c r="A5" t="s">
         <v>5</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="2">
         <v>0</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="2">
         <v>0.12296490988614681</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="2">
         <v>1.7486934390646469</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="2">
         <v>2.4117076579132268</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="2">
         <v>2.6457967397043669</v>
       </c>
       <c r="G5">
@@ -29455,19 +29492,19 @@
       <c r="A6" t="s">
         <v>6</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="2">
         <v>10</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="2">
         <v>0.1154047253544927</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="2">
         <v>1.7486934390646469</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="2">
         <v>2.4117076579132268</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="2">
         <v>2.6457967397043669</v>
       </c>
       <c r="G6">
@@ -29487,19 +29524,19 @@
       <c r="A7" t="s">
         <v>7</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="2">
         <v>52</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="2">
         <v>0.72313390895840146</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="2">
         <v>2.2670265825556322</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="2">
         <v>2.8009654597841389</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="2">
         <v>2.9916634021726218</v>
       </c>
       <c r="G7">
@@ -29519,19 +29556,19 @@
       <c r="A8" t="s">
         <v>8</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="2">
         <v>0</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="2">
         <v>3.8757615180228751</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="2">
         <v>5.8181815013320826</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="2">
         <v>5.8181829412644213</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="2">
         <v>5.8181818602198341</v>
       </c>
       <c r="G8">
@@ -29551,19 +29588,19 @@
       <c r="A9" t="s">
         <v>9</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="2">
         <v>0</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="2">
         <v>3.6374701851209359</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="2">
         <v>5.8181815013320826</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="2">
         <v>5.8181829412644213</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="2">
         <v>5.8181818602198341</v>
       </c>
       <c r="G9">
@@ -29583,19 +29620,19 @@
       <c r="A10" t="s">
         <v>10</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="2">
         <v>0</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="2">
         <v>3.4138295883574652</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="2">
         <v>5.8181815013320826</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="2">
         <v>5.8181829412644213</v>
       </c>
-      <c r="F10">
+      <c r="F10" s="2">
         <v>5.8181818602198341</v>
       </c>
       <c r="G10">
@@ -29615,19 +29652,19 @@
       <c r="A11" t="s">
         <v>11</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="2">
         <v>0</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="2">
         <v>3.2039389645079468</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="2">
         <v>5.8181815013320826</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="2">
         <v>5.8181829412644213</v>
       </c>
-      <c r="F11">
+      <c r="F11" s="2">
         <v>5.8181818602198341</v>
       </c>
       <c r="G11">
@@ -29647,19 +29684,19 @@
       <c r="A12" t="s">
         <v>12</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="2">
         <v>0</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="2">
         <v>3.0069529314822301</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="2">
         <v>5.8181815013320826</v>
       </c>
-      <c r="E12">
+      <c r="E12" s="2">
         <v>5.8181829412644213</v>
       </c>
-      <c r="F12">
+      <c r="F12" s="2">
         <v>5.8181818602198341</v>
       </c>
       <c r="G12">
@@ -29679,19 +29716,19 @@
       <c r="A13" t="s">
         <v>13</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="2">
         <v>10</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="2">
         <v>2.822078083356431</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="2">
         <v>5.8181815013320826</v>
       </c>
-      <c r="E13">
+      <c r="E13" s="2">
         <v>5.8181829412644213</v>
       </c>
-      <c r="F13">
+      <c r="F13" s="2">
         <v>5.8181818602198341</v>
       </c>
       <c r="G13">
@@ -29711,19 +29748,19 @@
       <c r="A14" t="s">
         <v>14</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="2">
         <v>0</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="2">
         <v>3.2633943441813691</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="2">
         <v>5.0842589437707293</v>
       </c>
-      <c r="E14">
+      <c r="E14" s="2">
         <v>5.2777292797224273</v>
       </c>
-      <c r="F14">
+      <c r="F14" s="2">
         <v>5.2857047909160864</v>
       </c>
       <c r="G14">
@@ -29743,19 +29780,19 @@
       <c r="A15" t="s">
         <v>15</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="2">
         <v>0</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="2">
         <v>3.0627528484537572</v>
       </c>
-      <c r="D15">
+      <c r="D15" s="2">
         <v>5.0842589437707293</v>
       </c>
-      <c r="E15">
+      <c r="E15" s="2">
         <v>5.2777292797224273</v>
       </c>
-      <c r="F15">
+      <c r="F15" s="2">
         <v>5.2857047909160864</v>
       </c>
       <c r="G15">
@@ -29775,19 +29812,19 @@
       <c r="A16" t="s">
         <v>16</v>
       </c>
-      <c r="B16">
+      <c r="B16" s="2">
         <v>0</v>
       </c>
-      <c r="C16">
+      <c r="C16" s="2">
         <v>2.87444728444693</v>
       </c>
-      <c r="D16">
+      <c r="D16" s="2">
         <v>5.0842589437707293</v>
       </c>
-      <c r="E16">
+      <c r="E16" s="2">
         <v>5.2777292797224273</v>
       </c>
-      <c r="F16">
+      <c r="F16" s="2">
         <v>5.2857047909160864</v>
       </c>
       <c r="G16">
@@ -29807,19 +29844,19 @@
       <c r="A17" t="s">
         <v>17</v>
       </c>
-      <c r="B17">
+      <c r="B17" s="2">
         <v>6</v>
       </c>
-      <c r="C17">
+      <c r="C17" s="2">
         <v>2.6977192087946822</v>
       </c>
-      <c r="D17">
+      <c r="D17" s="2">
         <v>5.0842589437707293</v>
       </c>
-      <c r="E17">
+      <c r="E17" s="2">
         <v>5.2777292797224273</v>
       </c>
-      <c r="F17">
+      <c r="F17" s="2">
         <v>5.2857047909160864</v>
       </c>
       <c r="G17">
@@ -29839,19 +29876,19 @@
       <c r="A18" t="s">
         <v>18</v>
       </c>
-      <c r="B18">
+      <c r="B18" s="2">
         <v>11</v>
       </c>
-      <c r="C18">
+      <c r="C18" s="2">
         <v>2.900751538749339</v>
       </c>
-      <c r="D18">
+      <c r="D18" s="2">
         <v>4.6353096263584623</v>
       </c>
-      <c r="E18">
+      <c r="E18" s="2">
         <v>4.8975760114134426</v>
       </c>
-      <c r="F18">
+      <c r="F18" s="2">
         <v>4.9189735974117426</v>
       </c>
       <c r="G18">
@@ -29871,19 +29908,19 @@
       <c r="A19" t="s">
         <v>19</v>
       </c>
-      <c r="B19">
+      <c r="B19" s="2">
         <v>0</v>
       </c>
-      <c r="C19">
+      <c r="C19" s="2">
         <v>3.3987132173409398</v>
       </c>
-      <c r="D19">
+      <c r="D19" s="2">
         <v>4.9457345297004798</v>
       </c>
-      <c r="E19">
+      <c r="E19" s="2">
         <v>5.1603971292890174</v>
       </c>
-      <c r="F19">
+      <c r="F19" s="2">
         <v>5.1726264350026909</v>
       </c>
       <c r="G19">
@@ -29903,19 +29940,19 @@
       <c r="A20" t="s">
         <v>20</v>
       </c>
-      <c r="B20">
+      <c r="B20" s="2">
         <v>2</v>
       </c>
-      <c r="C20">
+      <c r="C20" s="2">
         <v>3.1897519850913469</v>
       </c>
-      <c r="D20">
+      <c r="D20" s="2">
         <v>4.9457345297004798</v>
       </c>
-      <c r="E20">
+      <c r="E20" s="2">
         <v>5.1603971292890174</v>
       </c>
-      <c r="F20">
+      <c r="F20" s="2">
         <v>5.1726264350026909</v>
       </c>
       <c r="G20">
@@ -29935,19 +29972,19 @@
       <c r="A21" t="s">
         <v>21</v>
       </c>
-      <c r="B21">
+      <c r="B21" s="2">
         <v>52</v>
       </c>
-      <c r="C21">
+      <c r="C21" s="2">
         <v>3.1166031122745368</v>
       </c>
-      <c r="D21">
+      <c r="D21" s="2">
         <v>4.5952439271002419</v>
       </c>
-      <c r="E21">
+      <c r="E21" s="2">
         <v>4.8349094276150746</v>
       </c>
-      <c r="F21">
+      <c r="F21" s="2">
         <v>4.8689968785263469</v>
       </c>
       <c r="G21">
@@ -29967,19 +30004,19 @@
       <c r="A22" t="s">
         <v>22</v>
       </c>
-      <c r="B22">
+      <c r="B22" s="2">
         <v>18</v>
       </c>
-      <c r="C22">
+      <c r="C22" s="2">
         <v>6.1220743588884918</v>
       </c>
-      <c r="D22">
+      <c r="D22" s="2">
         <v>7.1456639132196829</v>
       </c>
-      <c r="E22">
+      <c r="E22" s="2">
         <v>7.1499883632326648</v>
       </c>
-      <c r="F22">
+      <c r="F22" s="2">
         <v>7.0448719878610211</v>
       </c>
       <c r="G22">
@@ -29999,19 +30036,19 @@
       <c r="A23" t="s">
         <v>23</v>
       </c>
-      <c r="B23">
+      <c r="B23" s="2">
         <v>6</v>
       </c>
-      <c r="C23">
+      <c r="C23" s="2">
         <v>6.8523583869353066</v>
       </c>
-      <c r="D23">
+      <c r="D23" s="2">
         <v>7.683723269288671</v>
       </c>
-      <c r="E23">
+      <c r="E23" s="2">
         <v>7.6306652836532001</v>
       </c>
-      <c r="F23">
+      <c r="F23" s="2">
         <v>7.5113716015734351</v>
       </c>
       <c r="G23">
@@ -30031,19 +30068,19 @@
       <c r="A24" t="s">
         <v>24</v>
       </c>
-      <c r="B24">
+      <c r="B24" s="2">
         <v>3</v>
       </c>
-      <c r="C24">
+      <c r="C24" s="2">
         <v>6.799953300815206</v>
       </c>
-      <c r="D24">
+      <c r="D24" s="2">
         <v>7.5250757462367428</v>
       </c>
-      <c r="E24">
+      <c r="E24" s="2">
         <v>7.4782617529234816</v>
       </c>
-      <c r="F24">
+      <c r="F24" s="2">
         <v>7.3864800401358108</v>
       </c>
       <c r="G24">
@@ -30063,19 +30100,19 @@
       <c r="A25" t="s">
         <v>25</v>
       </c>
-      <c r="B25">
+      <c r="B25" s="2">
         <v>1</v>
       </c>
-      <c r="C25">
+      <c r="C25" s="2">
         <v>6.5663228432120526</v>
       </c>
-      <c r="D25">
+      <c r="D25" s="2">
         <v>7.2083338760378624</v>
       </c>
-      <c r="E25">
+      <c r="E25" s="2">
         <v>7.1823847850985336</v>
       </c>
-      <c r="F25">
+      <c r="F25" s="2">
         <v>7.1256990992564768</v>
       </c>
       <c r="G25">
@@ -30095,19 +30132,19 @@
       <c r="A26" t="s">
         <v>26</v>
       </c>
-      <c r="B26">
+      <c r="B26" s="2">
         <v>0</v>
       </c>
-      <c r="C26">
+      <c r="C26" s="2">
         <v>6.2240916498056684</v>
       </c>
-      <c r="D26">
+      <c r="D26" s="2">
         <v>6.7974332172201963</v>
       </c>
-      <c r="E26">
+      <c r="E26" s="2">
         <v>6.8010934178726394</v>
       </c>
-      <c r="F26">
+      <c r="F26" s="2">
         <v>6.7829033795934048</v>
       </c>
       <c r="G26">
@@ -30127,19 +30164,19 @@
       <c r="A27" t="s">
         <v>27</v>
       </c>
-      <c r="B27">
+      <c r="B27" s="2">
         <v>4</v>
       </c>
-      <c r="C27">
+      <c r="C27" s="2">
         <v>5.8414192153849314</v>
       </c>
-      <c r="D27">
+      <c r="D27" s="2">
         <v>6.7974332172201963</v>
       </c>
-      <c r="E27">
+      <c r="E27" s="2">
         <v>6.8010934178726394</v>
       </c>
-      <c r="F27">
+      <c r="F27" s="2">
         <v>6.7829033795934048</v>
       </c>
       <c r="G27">
@@ -30159,19 +30196,19 @@
       <c r="A28" t="s">
         <v>28</v>
       </c>
-      <c r="B28">
+      <c r="B28" s="2">
         <v>10</v>
       </c>
-      <c r="C28">
+      <c r="C28" s="2">
         <v>5.7282042414437182</v>
       </c>
-      <c r="D28">
+      <c r="D28" s="2">
         <v>6.3773744841994091</v>
       </c>
-      <c r="E28">
+      <c r="E28" s="2">
         <v>6.4376901807625204</v>
       </c>
-      <c r="F28">
+      <c r="F28" s="2">
         <v>6.4474708022482821</v>
       </c>
       <c r="G28">
@@ -30191,19 +30228,19 @@
       <c r="A29" t="s">
         <v>29</v>
       </c>
-      <c r="B29">
+      <c r="B29" s="2">
         <v>0</v>
       </c>
-      <c r="C29">
+      <c r="C29" s="2">
         <v>5.9908447316951676</v>
       </c>
-      <c r="D29">
+      <c r="D29" s="2">
         <v>6.5295047573719494</v>
       </c>
-      <c r="E29">
+      <c r="E29" s="2">
         <v>6.5613884436520831</v>
       </c>
-      <c r="F29">
+      <c r="F29" s="2">
         <v>6.5706297313718824</v>
       </c>
       <c r="G29">
@@ -30223,19 +30260,19 @@
       <c r="A30" t="s">
         <v>30</v>
       </c>
-      <c r="B30">
+      <c r="B30" s="2">
         <v>0</v>
       </c>
-      <c r="C30">
+      <c r="C30" s="2">
         <v>5.622512890407771</v>
       </c>
-      <c r="D30">
+      <c r="D30" s="2">
         <v>6.5295047573719494</v>
       </c>
-      <c r="E30">
+      <c r="E30" s="2">
         <v>6.5613884436520831</v>
       </c>
-      <c r="F30">
+      <c r="F30" s="2">
         <v>6.5706297313718824</v>
       </c>
       <c r="G30">
@@ -30255,19 +30292,19 @@
       <c r="A31" t="s">
         <v>31</v>
       </c>
-      <c r="B31">
+      <c r="B31" s="2">
         <v>0</v>
       </c>
-      <c r="C31">
+      <c r="C31" s="2">
         <v>5.2768269949564264</v>
       </c>
-      <c r="D31">
+      <c r="D31" s="2">
         <v>6.5295047573719494</v>
       </c>
-      <c r="E31">
+      <c r="E31" s="2">
         <v>6.5613884436520831</v>
       </c>
-      <c r="F31">
+      <c r="F31" s="2">
         <v>6.5706297313718824</v>
       </c>
       <c r="G31">
@@ -30287,19 +30324,19 @@
       <c r="A32" t="s">
         <v>32</v>
       </c>
-      <c r="B32">
+      <c r="B32" s="2">
         <v>0</v>
       </c>
-      <c r="C32">
+      <c r="C32" s="2">
         <v>4.9523947169966247</v>
       </c>
-      <c r="D32">
+      <c r="D32" s="2">
         <v>6.5295047573719494</v>
       </c>
-      <c r="E32">
+      <c r="E32" s="2">
         <v>6.5613884436520831</v>
       </c>
-      <c r="F32">
+      <c r="F32" s="2">
         <v>6.5706297313718824</v>
       </c>
       <c r="G32">
@@ -30319,19 +30356,19 @@
       <c r="A33" t="s">
         <v>33</v>
       </c>
-      <c r="B33">
+      <c r="B33" s="2">
         <v>0</v>
       </c>
-      <c r="C33">
+      <c r="C33" s="2">
         <v>4.6479093319485649</v>
       </c>
-      <c r="D33">
+      <c r="D33" s="2">
         <v>6.5295047573719494</v>
       </c>
-      <c r="E33">
+      <c r="E33" s="2">
         <v>6.5613884436520831</v>
       </c>
-      <c r="F33">
+      <c r="F33" s="2">
         <v>6.5706297313718824</v>
       </c>
       <c r="G33">
@@ -30363,19 +30400,19 @@
       <c r="A34" t="s">
         <v>34</v>
       </c>
-      <c r="B34">
+      <c r="B34" s="2">
         <v>0</v>
       </c>
-      <c r="C34">
+      <c r="C34" s="2">
         <v>4.3621444558675471</v>
       </c>
-      <c r="D34">
+      <c r="D34" s="2">
         <v>6.5295047573719494</v>
       </c>
-      <c r="E34">
+      <c r="E34" s="2">
         <v>6.5613884436520831</v>
       </c>
-      <c r="F34">
+      <c r="F34" s="2">
         <v>6.5706297313718824</v>
       </c>
       <c r="G34">
@@ -30407,19 +30444,19 @@
       <c r="A35" t="s">
         <v>35</v>
       </c>
-      <c r="B35">
+      <c r="B35" s="2">
         <v>0</v>
       </c>
-      <c r="C35">
+      <c r="C35" s="2">
         <v>4.0939491059044943</v>
       </c>
-      <c r="D35">
+      <c r="D35" s="2">
         <v>6.5295047573719494</v>
       </c>
-      <c r="E35">
+      <c r="E35" s="2">
         <v>6.5613884436520831</v>
       </c>
-      <c r="F35">
+      <c r="F35" s="2">
         <v>6.5706297313718824</v>
       </c>
       <c r="G35">
@@ -30454,19 +30491,19 @@
       <c r="A36" t="s">
         <v>36</v>
       </c>
-      <c r="B36">
+      <c r="B36" s="2">
         <v>11</v>
       </c>
-      <c r="C36">
+      <c r="C36" s="2">
         <v>3.8422430644614849</v>
       </c>
-      <c r="D36">
+      <c r="D36" s="2">
         <v>6.5295047573719494</v>
       </c>
-      <c r="E36">
+      <c r="E36" s="2">
         <v>6.5613884436520831</v>
       </c>
-      <c r="F36">
+      <c r="F36" s="2">
         <v>6.5706297313718824</v>
       </c>
       <c r="G36">
@@ -30501,19 +30538,19 @@
       <c r="A37" t="s">
         <v>37</v>
       </c>
-      <c r="B37">
+      <c r="B37" s="2">
         <v>3</v>
       </c>
-      <c r="C37">
+      <c r="C37" s="2">
         <v>4.2823195327442027</v>
       </c>
-      <c r="D37">
+      <c r="D37" s="2">
         <v>5.4967807929184378</v>
       </c>
-      <c r="E37">
+      <c r="E37" s="2">
         <v>5.7425095750294766</v>
       </c>
-      <c r="F37">
+      <c r="F37" s="2">
         <v>5.7714957817339263</v>
       </c>
       <c r="G37">
@@ -30545,16 +30582,17 @@
       </c>
     </row>
     <row r="38" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="C38">
+      <c r="B38" s="2"/>
+      <c r="C38" s="2">
         <v>4.2034789999999997</v>
       </c>
-      <c r="D38">
+      <c r="D38" s="2">
         <v>5.3110229999999996</v>
       </c>
-      <c r="E38">
+      <c r="E38" s="2">
         <v>5.5485340000000001</v>
       </c>
-      <c r="F38">
+      <c r="F38" s="2">
         <v>5.5977540000000001</v>
       </c>
       <c r="L38" t="s">
@@ -30578,16 +30616,17 @@
       </c>
     </row>
     <row r="39" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="C39">
+      <c r="B39" s="2"/>
+      <c r="C39" s="2">
         <v>4.2034789999999997</v>
       </c>
-      <c r="D39">
+      <c r="D39" s="2">
         <v>5.3110229999999996</v>
       </c>
-      <c r="E39">
+      <c r="E39" s="2">
         <v>5.5485340000000001</v>
       </c>
-      <c r="F39">
+      <c r="F39" s="2">
         <v>5.5977540000000001</v>
       </c>
       <c r="L39" s="11"/>
@@ -30597,16 +30636,17 @@
       <c r="P39" s="11"/>
     </row>
     <row r="40" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="C40">
+      <c r="B40" s="2"/>
+      <c r="C40" s="2">
         <v>4.2034789999999997</v>
       </c>
-      <c r="D40">
+      <c r="D40" s="2">
         <v>5.3110229999999996</v>
       </c>
-      <c r="E40">
+      <c r="E40" s="2">
         <v>5.5485340000000001</v>
       </c>
-      <c r="F40">
+      <c r="F40" s="2">
         <v>5.5977540000000001</v>
       </c>
       <c r="L40" s="3"/>
@@ -30616,16 +30656,17 @@
       <c r="P40" s="4"/>
     </row>
     <row r="41" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="C41">
+      <c r="B41" s="2"/>
+      <c r="C41" s="2">
         <v>4.2034789999999997</v>
       </c>
-      <c r="D41">
+      <c r="D41" s="2">
         <v>5.3110229999999996</v>
       </c>
-      <c r="E41">
+      <c r="E41" s="2">
         <v>5.5485340000000001</v>
       </c>
-      <c r="F41">
+      <c r="F41" s="2">
         <v>5.5977540000000001</v>
       </c>
       <c r="L41" s="3"/>
@@ -30635,16 +30676,17 @@
       <c r="P41" s="4"/>
     </row>
     <row r="42" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="C42">
+      <c r="B42" s="2"/>
+      <c r="C42" s="2">
         <v>4.2034789999999997</v>
       </c>
-      <c r="D42">
+      <c r="D42" s="2">
         <v>5.3110229999999996</v>
       </c>
-      <c r="E42">
+      <c r="E42" s="2">
         <v>5.5485340000000001</v>
       </c>
-      <c r="F42">
+      <c r="F42" s="2">
         <v>5.5977540000000001</v>
       </c>
       <c r="L42" s="3"/>
@@ -30815,8 +30857,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="R42" sqref="R42"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="N48" sqref="N48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -32275,8 +32317,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection sqref="A1:D42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -32360,10 +32402,10 @@
       <c r="B6">
         <v>10</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="2">
         <v>1.0783389999999999</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="2">
         <v>0</v>
       </c>
       <c r="U6" s="8"/>
@@ -32375,10 +32417,10 @@
       <c r="B7">
         <v>52</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="2">
         <v>1.0783389999999999</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="2">
         <v>0</v>
       </c>
       <c r="U7" s="8"/>
@@ -32390,10 +32432,10 @@
       <c r="B8">
         <v>0</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="2">
         <v>6.1666910000000001</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="2">
         <v>5.852176</v>
       </c>
       <c r="U8" s="8"/>
@@ -32405,10 +32447,10 @@
       <c r="B9">
         <v>0</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="2">
         <v>6.1666910000000001</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="2">
         <v>5.852176</v>
       </c>
       <c r="U9" s="8"/>
@@ -32420,10 +32462,10 @@
       <c r="B10">
         <v>0</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="2">
         <v>6.1666910000000001</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="2">
         <v>6.147691</v>
       </c>
       <c r="U10" s="8"/>
@@ -32435,10 +32477,10 @@
       <c r="B11">
         <v>0</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="2">
         <v>6.1666910000000001</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="2">
         <v>6.1698870000000001</v>
       </c>
       <c r="U11" s="8"/>
@@ -32450,10 +32492,10 @@
       <c r="B12">
         <v>0</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="2">
         <v>6.1666910000000001</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="2">
         <v>6.1698870000000001</v>
       </c>
       <c r="U12" s="8"/>
@@ -32465,10 +32507,10 @@
       <c r="B13">
         <v>10</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="2">
         <v>6.1666910000000001</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="2">
         <v>6.1698870000000001</v>
       </c>
       <c r="U13" s="8"/>
@@ -32480,10 +32522,10 @@
       <c r="B14">
         <v>0</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="2">
         <v>5.1895519999999999</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="2">
         <v>5.6762990000000002</v>
       </c>
       <c r="U14" s="8"/>
@@ -32495,10 +32537,10 @@
       <c r="B15">
         <v>0</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="2">
         <v>5.1895519999999999</v>
       </c>
-      <c r="D15">
+      <c r="D15" s="2">
         <v>5.6762990000000002</v>
       </c>
       <c r="U15" s="8"/>
@@ -32510,10 +32552,10 @@
       <c r="B16">
         <v>0</v>
       </c>
-      <c r="C16">
+      <c r="C16" s="2">
         <v>5.1895519999999999</v>
       </c>
-      <c r="D16">
+      <c r="D16" s="2">
         <v>5.6762990000000002</v>
       </c>
       <c r="U16" s="8"/>
@@ -32525,10 +32567,10 @@
       <c r="B17">
         <v>6</v>
       </c>
-      <c r="C17">
+      <c r="C17" s="2">
         <v>5.1895519999999999</v>
       </c>
-      <c r="D17">
+      <c r="D17" s="2">
         <v>5.6269609999999997</v>
       </c>
       <c r="U17" s="8"/>
@@ -32540,10 +32582,10 @@
       <c r="B18">
         <v>11</v>
       </c>
-      <c r="C18">
+      <c r="C18" s="2">
         <v>4.4738360000000004</v>
       </c>
-      <c r="D18">
+      <c r="D18" s="2">
         <v>5.2961749999999999</v>
       </c>
       <c r="U18" s="8"/>
@@ -32555,10 +32597,10 @@
       <c r="B19">
         <v>0</v>
       </c>
-      <c r="C19">
+      <c r="C19" s="2">
         <v>4.4738360000000004</v>
       </c>
-      <c r="D19">
+      <c r="D19" s="2">
         <v>5.3348389999999997</v>
       </c>
       <c r="U19" s="8"/>
@@ -32570,10 +32612,10 @@
       <c r="B20">
         <v>2</v>
       </c>
-      <c r="C20">
+      <c r="C20" s="2">
         <v>4.5093719999999999</v>
       </c>
-      <c r="D20">
+      <c r="D20" s="2">
         <v>5.2795180000000004</v>
       </c>
       <c r="U20" s="8"/>
@@ -32585,10 +32627,10 @@
       <c r="B21">
         <v>52</v>
       </c>
-      <c r="C21">
+      <c r="C21" s="2">
         <v>4.5093719999999999</v>
       </c>
-      <c r="D21">
+      <c r="D21" s="2">
         <v>5.2196829999999999</v>
       </c>
       <c r="U21" s="8"/>
@@ -32600,10 +32642,10 @@
       <c r="B22">
         <v>18</v>
       </c>
-      <c r="C22">
+      <c r="C22" s="2">
         <v>7.6817570000000002</v>
       </c>
-      <c r="D22">
+      <c r="D22" s="2">
         <v>6.2039920000000004</v>
       </c>
       <c r="U22" s="8"/>
@@ -32615,10 +32657,10 @@
       <c r="B23">
         <v>6</v>
       </c>
-      <c r="C23">
+      <c r="C23" s="2">
         <v>7.6817570000000002</v>
       </c>
-      <c r="D23">
+      <c r="D23" s="2">
         <v>6.997306</v>
       </c>
       <c r="I23" t="s">
@@ -32636,10 +32678,10 @@
       <c r="B24">
         <v>3</v>
       </c>
-      <c r="C24">
+      <c r="C24" s="2">
         <v>8.1427560000000003</v>
       </c>
-      <c r="D24">
+      <c r="D24" s="2">
         <v>7.0972309999999998</v>
       </c>
       <c r="H24" t="s">
@@ -32660,10 +32702,10 @@
       <c r="B25">
         <v>1</v>
       </c>
-      <c r="C25">
+      <c r="C25" s="2">
         <v>8.1427560000000003</v>
       </c>
-      <c r="D25">
+      <c r="D25" s="2">
         <v>7.0252790000000003</v>
       </c>
       <c r="H25" t="s">
@@ -32684,10 +32726,10 @@
       <c r="B26">
         <v>0</v>
       </c>
-      <c r="C26">
+      <c r="C26" s="2">
         <v>7.0483010000000004</v>
       </c>
-      <c r="D26">
+      <c r="D26" s="2">
         <v>6.5723950000000002</v>
       </c>
       <c r="H26" t="s">
@@ -32708,10 +32750,10 @@
       <c r="B27">
         <v>4</v>
       </c>
-      <c r="C27">
+      <c r="C27" s="2">
         <v>7.0483010000000004</v>
       </c>
-      <c r="D27">
+      <c r="D27" s="2">
         <v>6.5723950000000002</v>
       </c>
       <c r="H27" t="s">
@@ -32734,10 +32776,10 @@
       <c r="B28">
         <v>10</v>
       </c>
-      <c r="C28">
+      <c r="C28" s="2">
         <v>6.1401979999999998</v>
       </c>
-      <c r="D28">
+      <c r="D28" s="2">
         <v>6.3916950000000003</v>
       </c>
       <c r="H28" s="11" t="s">
@@ -32754,10 +32796,10 @@
       <c r="B29">
         <v>0</v>
       </c>
-      <c r="C29">
+      <c r="C29" s="2">
         <v>6.1401979999999998</v>
       </c>
-      <c r="D29">
+      <c r="D29" s="2">
         <v>6.3611769999999996</v>
       </c>
       <c r="H29" s="3" t="s">
@@ -32777,10 +32819,10 @@
       <c r="B30">
         <v>0</v>
       </c>
-      <c r="C30">
+      <c r="C30" s="2">
         <v>5.84375</v>
       </c>
-      <c r="D30">
+      <c r="D30" s="2">
         <v>5.9639629999999997</v>
       </c>
       <c r="H30" s="3" t="s">
@@ -32800,10 +32842,10 @@
       <c r="B31">
         <v>0</v>
       </c>
-      <c r="C31">
+      <c r="C31" s="2">
         <v>5.84375</v>
       </c>
-      <c r="D31">
+      <c r="D31" s="2">
         <v>5.9229510000000003</v>
       </c>
       <c r="H31" s="12" t="s">
@@ -32820,10 +32862,10 @@
       <c r="B32">
         <v>0</v>
       </c>
-      <c r="C32">
+      <c r="C32" s="2">
         <v>5.84375</v>
       </c>
-      <c r="D32">
+      <c r="D32" s="2">
         <v>5.9229510000000003</v>
       </c>
       <c r="H32" s="3" t="s">
@@ -32843,10 +32885,10 @@
       <c r="B33">
         <v>0</v>
       </c>
-      <c r="C33">
+      <c r="C33" s="2">
         <v>5.84375</v>
       </c>
-      <c r="D33">
+      <c r="D33" s="2">
         <v>5.8846999999999996</v>
       </c>
       <c r="H33" s="3" t="s">
@@ -32866,10 +32908,10 @@
       <c r="B34">
         <v>0</v>
       </c>
-      <c r="C34">
+      <c r="C34" s="2">
         <v>5.84375</v>
       </c>
-      <c r="D34">
+      <c r="D34" s="2">
         <v>5.8846999999999996</v>
       </c>
       <c r="U34" s="8"/>
@@ -32881,10 +32923,10 @@
       <c r="B35">
         <v>0</v>
       </c>
-      <c r="C35">
+      <c r="C35" s="2">
         <v>5.84375</v>
       </c>
-      <c r="D35">
+      <c r="D35" s="2">
         <v>5.8846999999999996</v>
       </c>
       <c r="U35" s="8"/>
@@ -32896,10 +32938,10 @@
       <c r="B36">
         <v>11</v>
       </c>
-      <c r="C36">
+      <c r="C36" s="2">
         <v>5.84375</v>
       </c>
-      <c r="D36">
+      <c r="D36" s="2">
         <v>5.8846999999999996</v>
       </c>
       <c r="U36" s="8"/>
@@ -32911,10 +32953,10 @@
       <c r="B37">
         <v>3</v>
       </c>
-      <c r="C37">
+      <c r="C37" s="2">
         <v>5.84375</v>
       </c>
-      <c r="D37">
+      <c r="D37" s="2">
         <v>5.6992289999999999</v>
       </c>
       <c r="H37" s="3"/>
@@ -32923,10 +32965,10 @@
       <c r="U37" s="8"/>
     </row>
     <row r="38" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="C38">
+      <c r="C38" s="2">
         <v>4.9694890000000003</v>
       </c>
-      <c r="D38">
+      <c r="D38" s="2">
         <v>4.8929150000000003</v>
       </c>
       <c r="H38" s="3"/>
@@ -32935,35 +32977,35 @@
       <c r="U38" s="8"/>
     </row>
     <row r="39" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="C39">
+      <c r="C39" s="2">
         <v>4.9694890000000003</v>
       </c>
-      <c r="D39">
+      <c r="D39" s="2">
         <v>4.8929150000000003</v>
       </c>
       <c r="U39" s="8"/>
     </row>
     <row r="40" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="C40">
+      <c r="C40" s="2">
         <v>4.9694890000000003</v>
       </c>
-      <c r="D40">
+      <c r="D40" s="2">
         <v>4.8929150000000003</v>
       </c>
     </row>
     <row r="41" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="C41">
+      <c r="C41" s="2">
         <v>4.9694890000000003</v>
       </c>
-      <c r="D41">
+      <c r="D41" s="2">
         <v>4.8929150000000003</v>
       </c>
     </row>
     <row r="42" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="C42">
+      <c r="C42" s="2">
         <v>4.9694890000000003</v>
       </c>
-      <c r="D42">
+      <c r="D42" s="2">
         <v>4.8929150000000003</v>
       </c>
     </row>

</xml_diff>